<commit_message>
se agregó la capitalizacion.
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9264" activeTab="3"/>
+    <workbookView windowWidth="10848" windowHeight="9120" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="formula ganancias" sheetId="1" r:id="rId1"/>
@@ -2493,8 +2493,8 @@
   <sheetPr/>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2546,21 +2546,21 @@
         <v>11</v>
       </c>
       <c r="E3" s="11">
-        <v>4.8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="12">
-        <v>4</v>
+        <v>4.302</v>
       </c>
       <c r="G3" s="13">
         <f t="shared" ref="G3:G17" si="0">E3*F3</f>
-        <v>19.2</v>
+        <v>30.114</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="25">
         <f>IF(B1="BUY",(J10/I10)-1,(I10/J10)-1)*100</f>
-        <v>-1.93647182589129</v>
+        <v>-1.71194044216326</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:10">
@@ -2575,23 +2575,21 @@
         <v>1</v>
       </c>
       <c r="E4" s="15">
-        <f>E3*(1+$B$6/100)</f>
-        <v>6.24</v>
+        <v>9</v>
       </c>
       <c r="F4" s="16">
-        <f>F3*(1-$B$5/100)</f>
-        <v>3.932</v>
+        <v>4.229</v>
       </c>
       <c r="G4" s="17">
         <f t="shared" si="0"/>
-        <v>24.53568</v>
+        <v>38.061</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="25">
         <f>E18</f>
-        <v>458.06766144</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:10">
@@ -2605,23 +2603,21 @@
         <v>2</v>
       </c>
       <c r="E5" s="15">
-        <f>E4*(1+$B$6/100)</f>
-        <v>8.112</v>
+        <v>11</v>
       </c>
       <c r="F5" s="16">
-        <f t="shared" ref="F5:F10" si="1">F4*(1-$B$5/100)</f>
-        <v>3.865156</v>
+        <v>4.156</v>
       </c>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
-        <v>31.354145472</v>
+        <v>45.716</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="25">
         <f>J4*J10</f>
-        <v>1588.94091944911</v>
+        <v>1801.455453</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:10">
@@ -2635,23 +2631,21 @@
         <v>3</v>
       </c>
       <c r="E6" s="15">
-        <f>E5*(1+$B$6/100)</f>
-        <v>10.5456</v>
+        <v>15</v>
       </c>
       <c r="F6" s="16">
-        <f t="shared" si="1"/>
-        <v>3.799448348</v>
+        <v>4.083</v>
       </c>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
-        <v>40.0674624986688</v>
+        <v>61.245</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="25">
         <f>J3/100*J4*J10</f>
-        <v>-30.7693932351901</v>
+        <v>-30.8398444474624</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:7">
@@ -2665,16 +2659,14 @@
         <v>4</v>
       </c>
       <c r="E7" s="15">
-        <f>E6*(1+$B$6/100)</f>
-        <v>13.70928</v>
+        <v>19</v>
       </c>
       <c r="F7" s="16">
-        <f t="shared" si="1"/>
-        <v>3.734857726084</v>
+        <v>4.009</v>
       </c>
       <c r="G7" s="17">
         <f t="shared" si="0"/>
-        <v>51.2022103270489</v>
+        <v>76.171</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:7">
@@ -2683,22 +2675,20 @@
       </c>
       <c r="B8" s="9">
         <f>(LOG10((B4+G18)/(E18*F3))/LOG10(1-(B5/100)))</f>
-        <v>8.31021590397248</v>
+        <v>7.47384205143812</v>
       </c>
       <c r="D8" s="14">
         <v>5</v>
       </c>
       <c r="E8" s="15">
-        <f>E7*(1+$B$6/100)</f>
-        <v>17.822064</v>
+        <v>25</v>
       </c>
       <c r="F8" s="16">
-        <f t="shared" si="1"/>
-        <v>3.67136514474057</v>
+        <v>3.936</v>
       </c>
       <c r="G8" s="17">
         <f t="shared" si="0"/>
-        <v>65.4313045769357</v>
+        <v>98.4</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:10">
@@ -2713,16 +2703,14 @@
         <v>6</v>
       </c>
       <c r="E9" s="15">
-        <f>E8*(1+$B$6/100)</f>
-        <v>23.1686832</v>
+        <v>33</v>
       </c>
       <c r="F9" s="16">
-        <f t="shared" si="1"/>
-        <v>3.60895193727998</v>
+        <v>3.863</v>
       </c>
       <c r="G9" s="19">
         <f t="shared" si="0"/>
-        <v>83.6146641188662</v>
+        <v>127.479</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>24</v>
@@ -2735,25 +2723,19 @@
       <c r="D10" s="14">
         <v>7</v>
       </c>
-      <c r="E10" s="15">
-        <f>E9*(1+$B$6/100)</f>
-        <v>30.11928816</v>
-      </c>
-      <c r="F10" s="16">
-        <f t="shared" si="1"/>
-        <v>3.54759975434622</v>
-      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="19">
         <f t="shared" si="0"/>
-        <v>106.851179277499</v>
+        <v>0</v>
       </c>
       <c r="I10" s="26">
         <f>G18/E18</f>
-        <v>3.53728947892853</v>
+        <v>3.85048834663866</v>
       </c>
       <c r="J10" s="27">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>3.46879086476886</v>
+        <v>3.78457027941176</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="4:7">
@@ -2828,27 +2810,27 @@
       </c>
       <c r="E17" s="21">
         <f>SUM(E3:E15)*3</f>
-        <v>343.55074608</v>
+        <v>357</v>
       </c>
       <c r="F17" s="22">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-$B$5/100),MAX(F3:F16)*(1+$B$5/100))</f>
-        <v>3.48729055852234</v>
+        <v>3.797329</v>
       </c>
       <c r="G17" s="23">
         <f t="shared" si="0"/>
-        <v>1198.06127317809</v>
+        <v>1355.646453</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:8">
       <c r="D18" s="3"/>
       <c r="E18" s="24">
         <f>SUM(E3:E17)</f>
-        <v>458.06766144</v>
+        <v>476</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="24">
         <f>SUM(G3:G17)</f>
-        <v>1620.31791944911</v>
+        <v>1832.832453</v>
       </c>
       <c r="H18" s="3"/>
     </row>

</xml_diff>

<commit_message>
mejora para cancelar stopvelavela
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -1705,7 +1705,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -1751,21 +1751,21 @@
         <v>11</v>
       </c>
       <c r="B3" s="20">
-        <v>320.11</v>
+        <v>320.28</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="22">
         <f>G3/F3</f>
-        <v>3518.33669170178</v>
+        <v>3520.20516578128</v>
       </c>
       <c r="F3" s="23">
         <v>0.005459</v>
       </c>
       <c r="G3" s="24">
         <f>B8</f>
-        <v>19.2066</v>
+        <v>19.2168</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>13</v>
@@ -1781,14 +1781,14 @@
       </c>
       <c r="B4" s="6">
         <f>-B3*$B$19/100</f>
-        <v>-32.011</v>
+        <v>-32.028</v>
       </c>
       <c r="D4" s="25">
         <v>1</v>
       </c>
       <c r="E4" s="26">
         <f>E3*(1+$B$6/100)</f>
-        <v>4573.83769921231</v>
+        <v>4576.26671551566</v>
       </c>
       <c r="F4" s="27">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
@@ -1796,14 +1796,14 @@
       </c>
       <c r="G4" s="24">
         <f t="shared" ref="G4:G16" si="0">E4*F4</f>
-        <v>24.54411414</v>
+        <v>24.55714872</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="36">
         <f>E18</f>
-        <v>450558.167326035</v>
+        <v>450797.444101035</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:10">
@@ -1817,23 +1817,23 @@
         <v>2</v>
       </c>
       <c r="E5" s="26">
-        <f t="shared" ref="E5:E16" si="1">E4*(1+$B$6/100)</f>
-        <v>5945.989008976</v>
+        <f>E4*(1+$B$6/100)</f>
+        <v>5949.14673017036</v>
       </c>
       <c r="F5" s="27">
-        <f t="shared" ref="F5:F12" si="2">IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
+        <f t="shared" ref="F5:F12" si="1">IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
         <v>0.005274971651</v>
       </c>
       <c r="G5" s="24">
         <f t="shared" si="0"/>
-        <v>31.364923459506</v>
+        <v>31.381580349288</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J5" s="36">
         <f>J4*J10</f>
-        <v>2126.11872865713</v>
+        <v>2127.24784109933</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:10">
@@ -1847,23 +1847,23 @@
         <v>3</v>
       </c>
       <c r="E6" s="26">
+        <f>E5*(1+$B$6/100)</f>
+        <v>7733.89074922147</v>
+      </c>
+      <c r="F6" s="27">
         <f t="shared" si="1"/>
-        <v>7729.78571166881</v>
-      </c>
-      <c r="F6" s="27">
-        <f t="shared" si="2"/>
         <v>0.005185297132933</v>
       </c>
       <c r="G6" s="24">
         <f t="shared" si="0"/>
-        <v>40.0812356889027</v>
+        <v>40.1025215283551</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="36">
         <f>J3/100*J4*J10</f>
-        <v>-31.5361888209531</v>
+        <v>-31.5529366641931</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:10">
@@ -1877,16 +1877,16 @@
         <v>4</v>
       </c>
       <c r="E7" s="26">
+        <f>E6*(1+$B$6/100)</f>
+        <v>10054.0579739879</v>
+      </c>
+      <c r="F7" s="27">
         <f t="shared" si="1"/>
-        <v>10048.7214251694</v>
-      </c>
-      <c r="F7" s="27">
-        <f t="shared" si="2"/>
         <v>0.00509714708167314</v>
       </c>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>51.2198110868488</v>
+        <v>51.247012261085</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>21</v>
@@ -1902,22 +1902,22 @@
       </c>
       <c r="B8" s="6">
         <f>B3*$B$18/100</f>
-        <v>19.2066</v>
+        <v>19.2168</v>
       </c>
       <c r="D8" s="25">
         <v>5</v>
       </c>
       <c r="E8" s="26">
+        <f>E7*(1+$B$6/100)</f>
+        <v>13070.2753661843</v>
+      </c>
+      <c r="F8" s="27">
         <f t="shared" si="1"/>
-        <v>13063.3378527203</v>
-      </c>
-      <c r="F8" s="27">
-        <f t="shared" si="2"/>
         <v>0.0050104955812847</v>
       </c>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>65.4537965878841</v>
+        <v>65.4885569684405</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:10">
@@ -1931,16 +1931,16 @@
         <v>6</v>
       </c>
       <c r="E9" s="26">
+        <f>E8*(1+$B$6/100)</f>
+        <v>16991.3579760396</v>
+      </c>
+      <c r="F9" s="27">
         <f t="shared" si="1"/>
-        <v>16982.3392085364</v>
-      </c>
-      <c r="F9" s="27">
-        <f t="shared" si="2"/>
         <v>0.00492531715640286</v>
       </c>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>83.6434066596571</v>
+        <v>83.6878269499702</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>24</v>
@@ -1955,22 +1955,22 @@
       </c>
       <c r="B10" s="29">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$E$3</f>
-        <v>112639.541831509</v>
+        <v>112699.361025259</v>
       </c>
       <c r="D10" s="25">
         <v>7</v>
       </c>
       <c r="E10" s="26">
-        <f t="shared" si="1"/>
-        <v>22077.0409710973</v>
+        <f>E9*(1+$B$6/100)</f>
+        <v>22088.7653688514</v>
       </c>
       <c r="F10" s="27">
-        <f t="shared" si="2"/>
+        <f>IF($B$1="BUY",F9*(1-$B$5/100),F9*(1+$B$5/100))</f>
         <v>0.00484158676474401</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>106.887909370376</v>
+        <v>106.944674059367</v>
       </c>
       <c r="I10" s="37">
         <f>G18/E18</f>
@@ -1987,22 +1987,22 @@
       </c>
       <c r="B11" s="29">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$G$3</f>
-        <v>614.899258858206</v>
+        <v>615.225811836888</v>
       </c>
       <c r="D11" s="25">
         <v>8</v>
       </c>
       <c r="E11" s="26">
-        <f t="shared" si="1"/>
-        <v>28700.1532624265</v>
+        <f>E10*(1+$B$6/100)</f>
+        <v>28715.3949795069</v>
       </c>
       <c r="F11" s="27">
-        <f t="shared" si="2"/>
+        <f>IF($B$1="BUY",F10*(1-$B$5/100),F10*(1+$B$5/100))</f>
         <v>0.00475927978974336</v>
       </c>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>136.592059384403</v>
+        <v>136.664598980465</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:7">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B12" s="29">
         <f>B10*3</f>
-        <v>337918.625494526</v>
+        <v>338098.083075777</v>
       </c>
       <c r="D12" s="25">
         <v>9</v>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B13" s="29">
         <f>B11*3</f>
-        <v>1844.69777657462</v>
+        <v>1845.67743551066</v>
       </c>
       <c r="D13" s="25">
         <v>10</v>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B14" s="29">
         <f>B12+B10</f>
-        <v>450558.167326035</v>
+        <v>450797.444101035</v>
       </c>
       <c r="D14" s="25">
         <v>11</v>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B15" s="29">
         <f>B13+B11</f>
-        <v>2459.59703543282</v>
+        <v>2460.90324734755</v>
       </c>
       <c r="D15" s="25">
         <v>12</v>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="E17" s="31">
         <f>SUM(E3:E15)*3</f>
-        <v>337918.625494526</v>
+        <v>338098.083075777</v>
       </c>
       <c r="F17" s="32">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="G17" s="33">
         <f>E17*F17</f>
-        <v>1599.13587227955</v>
+        <v>1599.98512128236</v>
       </c>
       <c r="J17" s="39"/>
     </row>
@@ -2130,12 +2130,12 @@
       <c r="D18" s="2"/>
       <c r="E18" s="35">
         <f>SUM(E3:E17)</f>
-        <v>450558.167326035</v>
+        <v>450797.444101035</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35">
         <f>SUM(G3:G17)</f>
-        <v>2158.12972865713</v>
+        <v>2159.27584109933</v>
       </c>
       <c r="H18" s="2"/>
       <c r="J18" s="39"/>

</xml_diff>

<commit_message>
se prueba con porcentaje de entrada de 10
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>SALDO INICIAL</t>
   </si>
@@ -163,10 +163,10 @@
     <t>Ataque</t>
   </si>
   <si>
-    <t>suma total de cantidad según el número de compensaciones</t>
-  </si>
-  <si>
     <t>Soporta una varación en contra %</t>
+  </si>
+  <si>
+    <t>va 6. Probando 10</t>
   </si>
   <si>
     <t>peor de los casos</t>
@@ -183,12 +183,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.00000"/>
-    <numFmt numFmtId="179" formatCode="0.0000_ "/>
+    <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -246,16 +246,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,13 +268,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -283,23 +275,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,7 +290,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -369,14 +361,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -384,13 +369,28 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +411,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -429,49 +435,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,13 +591,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,109 +603,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -874,30 +880,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -975,16 +957,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -999,131 +1005,131 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1149,28 +1155,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1179,28 +1188,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1215,25 +1224,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1242,25 +1251,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1698,78 +1713,78 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="20.5740740740741" style="47" customWidth="1"/>
-    <col min="2" max="2" width="34.287037037037" style="47" customWidth="1"/>
-    <col min="3" max="3" width="14.1481481481481" style="48" customWidth="1"/>
+    <col min="1" max="1" width="20.5740740740741" style="50" customWidth="1"/>
+    <col min="2" max="2" width="34.287037037037" style="50" customWidth="1"/>
+    <col min="3" max="3" width="14.1481481481481" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A2" s="51">
+      <c r="A2" s="54">
         <v>449.74</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="55">
         <v>1</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="54">
         <v>30</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="52" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A5" s="52">
+      <c r="A5" s="55">
         <f>POWER(1+(B2/100),C2)*A2</f>
         <v>606.181571181821</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="55">
         <f>A5-A2</f>
         <v>156.441571181821</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="55"/>
+      <c r="B7" s="58"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="56" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="53">
+      <c r="A9" s="56">
         <v>3</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="56">
         <f>A9*100/A2</f>
         <v>0.667052074531952</v>
       </c>
@@ -1841,11 +1856,11 @@
       <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="46">
         <f>G3/F3</f>
         <v>3607.69371679795</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="47">
         <v>0.005459</v>
       </c>
       <c r="G3" s="13">
@@ -1855,7 +1870,7 @@
       <c r="I3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="25">
         <f>IF(B1="BUY",(J10/I10)-1,(I10/J10)-1)*100</f>
         <v>-1.1306113867434</v>
       </c>
@@ -1886,7 +1901,7 @@
       <c r="I4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="25">
         <f>E18</f>
         <v>462001.227212826</v>
       </c>
@@ -1916,7 +1931,7 @@
       <c r="I5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="25">
         <f>J4*J10</f>
         <v>2903.20797975916</v>
       </c>
@@ -1946,7 +1961,7 @@
       <c r="I6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="25">
         <f>J3/100*J4*J10</f>
         <v>-32.824</v>
       </c>
@@ -1976,7 +1991,7 @@
       <c r="I7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="18">
         <f>IF(B1="BUY",(J10/F3)-1,(F3/J10)-1)*100</f>
         <v>-13.1283491593311</v>
       </c>
@@ -2006,10 +2021,10 @@
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:10">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="49">
         <v>8</v>
       </c>
       <c r="D9" s="15">
@@ -2035,10 +2050,10 @@
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="17.4" spans="1:10">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="49">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$E$3</f>
         <v>115500.306803206</v>
       </c>
@@ -2057,20 +2072,20 @@
         <f t="shared" si="1"/>
         <v>139.057011276782</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="26">
         <f>G18/E18</f>
         <v>0.00621293583368965</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="27">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
         <v>0.00628398326401364</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:7">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="49">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$G$3</f>
         <v>630.516174838704</v>
       </c>
@@ -2091,10 +2106,10 @@
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:7">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="49">
         <f>B10*3</f>
         <v>346500.920409619</v>
       </c>
@@ -2109,10 +2124,10 @@
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:7">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="49">
         <f>B11*3</f>
         <v>1891.54852451611</v>
       </c>
@@ -2127,10 +2142,10 @@
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:7">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="49">
         <f>B12+B10</f>
         <v>462001.227212826</v>
       </c>
@@ -2145,10 +2160,10 @@
       </c>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:7">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="46">
+      <c r="B15" s="49">
         <f>B13+B11</f>
         <v>2522.06469935482</v>
       </c>
@@ -2163,10 +2178,10 @@
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:7">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="46">
+      <c r="B16" s="49">
         <f>B15/B14</f>
         <v>0.005459</v>
       </c>
@@ -2181,73 +2196,73 @@
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="18.15" spans="1:10">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="46">
+      <c r="B17" s="49">
         <f>IF(B1="BUY",((B4/B15)+1)*B16,((B4/-B15)+1)*B16)</f>
         <v>0.00553004743032399</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="20">
         <f>SUM(E3:E15)*3</f>
         <v>346500.920409619</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="21">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
         <v>0.0062825329229257</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="22">
         <f t="shared" si="1"/>
         <v>2176.90344029749</v>
       </c>
-      <c r="J17" s="31"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:10">
       <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="18">
         <v>6</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23">
+      <c r="D18" s="23"/>
+      <c r="E18" s="24">
         <f>SUM(E3:E17)</f>
         <v>462001.227212826</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23">
+      <c r="F18" s="24"/>
+      <c r="G18" s="24">
         <f>SUM(G3:G17)</f>
         <v>2870.38397975916</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="J18" s="31"/>
+      <c r="H18" s="23"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:10">
       <c r="A19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="18">
         <v>10</v>
       </c>
-      <c r="J19" s="31"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="10:10">
-      <c r="J20" s="31"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="10:10">
-      <c r="J21" s="31"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="31"/>
+      <c r="J22" s="32"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="31"/>
+      <c r="J23" s="32"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="31"/>
+      <c r="J24" s="32"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J6">
@@ -2322,20 +2337,20 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.5833333333333" customWidth="1"/>
-    <col min="2" max="2" width="12.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="8.44444444444444" customWidth="1"/>
-    <col min="5" max="5" width="8.66666666666667" customWidth="1"/>
-    <col min="6" max="6" width="10.4444444444444" customWidth="1"/>
-    <col min="7" max="7" width="9.9537037037037" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.787037037037" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.4444444444444" customWidth="1"/>
-    <col min="10" max="10" width="19.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="8.44444444444444" customWidth="1"/>
+    <col min="2" max="2" width="10.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="5.22222222222222" customWidth="1"/>
+    <col min="6" max="6" width="11.1111111111111" customWidth="1"/>
+    <col min="7" max="7" width="7.97222222222222" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.3333333333333" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.8888888888889" customWidth="1"/>
+    <col min="10" max="10" width="9.66666666666667" customWidth="1"/>
     <col min="11" max="11" width="9.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2352,31 +2367,31 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2384,38 +2399,38 @@
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34">
-        <v>513.22</v>
+      <c r="B3" s="35">
+        <v>519.93</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="36">
-        <v>200</v>
-      </c>
-      <c r="F3" s="37">
-        <v>4.7457</v>
-      </c>
-      <c r="G3" s="17">
-        <f>E3/F3</f>
-        <v>42.1434140379712</v>
-      </c>
-      <c r="H3" s="38">
+      <c r="E3" s="37">
+        <v>26.69</v>
+      </c>
+      <c r="F3" s="38">
+        <v>6.372</v>
+      </c>
+      <c r="G3" s="18">
+        <f t="shared" ref="G3:G6" si="0">E3/F3</f>
+        <v>4.18863779033271</v>
+      </c>
+      <c r="H3" s="39">
         <f>IF(A2="BUY",((I3/J3)-1)*-100,((I3/J3)-1)*100)</f>
-        <v>-20.6379333917757</v>
-      </c>
-      <c r="I3" s="38">
+        <v>-1.74784188103865</v>
+      </c>
+      <c r="I3" s="39">
         <f>SUM(E3:E4)/SUM(G3:G4)</f>
-        <v>4.6961185168188</v>
-      </c>
-      <c r="J3" s="40">
+        <v>4.70094248080813</v>
+      </c>
+      <c r="J3" s="42">
         <f>IF(A2="BUY",((B4/SUM(E3:E4))+1)*I3,((B4/-SUM(E3:E4))+1)*I3)</f>
-        <v>3.89273786841822</v>
-      </c>
-      <c r="K3" s="41">
+        <v>4.62018888450171</v>
+      </c>
+      <c r="K3" s="43">
         <f>H3/100*SUM(G3:G4)*J3</f>
-        <v>-51.322</v>
+        <v>-51.9930000000002</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2424,34 +2439,28 @@
       </c>
       <c r="B4" s="14">
         <f>-B3*10/100</f>
-        <v>-51.322</v>
+        <v>-51.993</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="36">
-        <v>100</v>
-      </c>
-      <c r="F4" s="37">
-        <v>4.6</v>
-      </c>
-      <c r="G4" s="17">
-        <f>E4/F4</f>
-        <v>21.7391304347826</v>
-      </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="42"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1.7</v>
-      </c>
+      <c r="E4" s="37">
+        <v>3000</v>
+      </c>
+      <c r="F4" s="38">
+        <v>4.69</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="0"/>
+        <v>639.658848614072</v>
+      </c>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="44"/>
+    </row>
+    <row r="5" spans="3:10">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2461,29 +2470,28 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="14">
-        <v>30</v>
-      </c>
+    <row r="6" spans="3:11">
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="14">
-        <v>10</v>
-      </c>
+      <c r="D6" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="18">
+        <f>IF(A2="BUY",((F3/J6)-1)*-100,((F3/J6)-1)*100)</f>
+        <v>3.45454545454545</v>
+      </c>
+      <c r="I6" s="41"/>
+      <c r="J6" s="38">
+        <v>6.6</v>
+      </c>
+      <c r="K6" s="45">
+        <f>H6/100*SUM(G3)*J6</f>
+        <v>0.955009416195857</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2492,15 +2500,9 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="14">
-        <f>B3*10/100</f>
-        <v>51.322</v>
-      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="3:11">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2509,14 +2511,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17">
-        <v>6</v>
-      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="3:10">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2526,14 +2523,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="17">
-        <f>((1-POWER(1+$B$6/100,B9+1))/(1-(1+$B$6/100)))*E3</f>
-        <v>3516.5678</v>
-      </c>
+    <row r="10" spans="3:10">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2587,15 +2577,15 @@
   <sheetPr/>
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="58.7777777777778" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.8888888888889" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8888888888889" style="1"/>
+    <col min="3" max="3" width="17.1111111111111" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.44444444444444" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.7777777777778" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
@@ -2636,28 +2626,28 @@
         <v>13</v>
       </c>
       <c r="B3" s="9">
-        <v>511.74</v>
+        <v>519.93</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="11">
         <f>G3/F3</f>
-        <v>5295.68816833391</v>
+        <v>8.81835142469471</v>
       </c>
       <c r="F3" s="12">
-        <v>0.005798</v>
+        <v>5.896</v>
       </c>
       <c r="G3" s="13">
         <f>B8</f>
-        <v>30.7044</v>
+        <v>51.993</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="25">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-20.7099083127727</v>
+        <v>-13.548279491961</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:10">
@@ -2666,29 +2656,29 @@
       </c>
       <c r="B4" s="14">
         <f>-B3*$B$10/100</f>
-        <v>-51.174</v>
+        <v>-51.993</v>
       </c>
       <c r="D4" s="15">
         <v>1</v>
       </c>
       <c r="E4" s="11">
         <f>E3*(1+$B$6/100)</f>
-        <v>6884.39461883408</v>
+        <v>11.4638568521031</v>
       </c>
       <c r="F4" s="16">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
-        <v>0.005896566</v>
+        <v>5.996232</v>
       </c>
       <c r="G4" s="13">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>40.59428724</v>
+        <v>68.7399453</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="25">
         <f>E18</f>
-        <v>32764.4226974819</v>
+        <v>54.5591402645862</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:10">
@@ -2703,22 +2693,22 @@
       </c>
       <c r="E5" s="11">
         <f>E4*(1+$B$6/100)</f>
-        <v>8949.71300448431</v>
+        <v>14.9030139077341</v>
       </c>
       <c r="F5" s="16">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
-        <v>0.005996807622</v>
+        <v>6.098167944</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="0"/>
-        <v>53.669707160004</v>
+        <v>90.88108168113</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="25">
         <f>J4*J10</f>
-        <v>247.099114236245</v>
+        <v>383.760905071752</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:10">
@@ -2733,22 +2723,22 @@
       </c>
       <c r="E6" s="11">
         <f>E5*(1+$B$6/100)</f>
-        <v>11634.6269058296</v>
+        <v>19.3739180800543</v>
       </c>
       <c r="F6" s="16">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
-        <v>0.006098753351574</v>
+        <v>6.201836799048</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="0"/>
-        <v>70.9567198362413</v>
+        <v>120.153878090622</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="25">
         <f>J3/100*J4*J10</f>
-        <v>-51.174</v>
+        <v>-51.993</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:10">
@@ -2768,11 +2758,11 @@
         <v>0</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="17">
+        <v>48</v>
+      </c>
+      <c r="J7" s="18">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>30.0739885166909</v>
+        <v>19.2987070124616</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:7">
@@ -2781,7 +2771,7 @@
       </c>
       <c r="B8" s="14">
         <f>B3*$B$9/100</f>
-        <v>30.7044</v>
+        <v>51.993</v>
       </c>
       <c r="D8" s="15">
         <v>5</v>
@@ -2798,7 +2788,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="17">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D9" s="15">
         <v>6</v>
@@ -2820,7 +2813,7 @@
       <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="18">
         <v>10</v>
       </c>
       <c r="D10" s="15">
@@ -2832,13 +2825,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="26">
         <f>G18/E18</f>
-        <v>0.0059798128001597</v>
-      </c>
-      <c r="J10" s="26">
+        <v>6.0808858692207</v>
+      </c>
+      <c r="J10" s="27">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>0.00754168985419774</v>
+        <v>7.03385176545474</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="4:7">
@@ -2873,10 +2866,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="27"/>
+      <c r="J13" s="28"/>
     </row>
     <row r="14" s="1" customFormat="1" spans="4:9">
       <c r="D14" s="15">
@@ -2888,7 +2881,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="29" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2902,9 +2895,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="18">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>0.00754168985419774</v>
+        <v>7.03385176545474</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="4:9">
@@ -2917,57 +2910,57 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="30" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="18.15" spans="4:10">
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20">
+      <c r="E17" s="20"/>
+      <c r="F17" s="21">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
-        <v>0.00613331295389958</v>
-      </c>
-      <c r="G17" s="21">
+        <v>6.23698054090927</v>
+      </c>
+      <c r="G17" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="18">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>26.1191630279183</v>
-      </c>
-      <c r="J17" s="30" t="str">
+        <v>15.671497816751</v>
+      </c>
+      <c r="J17" s="31" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
         <v>TIENE QUE BAJAR</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" spans="4:10">
-      <c r="D18" s="22"/>
-      <c r="E18" s="23">
+      <c r="D18" s="23"/>
+      <c r="E18" s="24">
         <f>SUM(E3:E17)</f>
-        <v>32764.4226974819</v>
-      </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23">
+        <v>54.5591402645862</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24">
         <f>SUM(G3:G17)</f>
-        <v>195.925114236245</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="J18" s="31"/>
+        <v>331.767905071752</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="10:10">
-      <c r="J19" s="31"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="10:10">
-      <c r="J20" s="31"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="10:10">
-      <c r="J21" s="31"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="10:16384">
-      <c r="J22" s="31"/>
+      <c r="J22" s="32"/>
       <c r="XEV22"/>
       <c r="XEW22"/>
       <c r="XEX22"/>
@@ -2979,7 +2972,7 @@
       <c r="XFD22"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="10:16384">
-      <c r="J23" s="31"/>
+      <c r="J23" s="32"/>
       <c r="XEV23"/>
       <c r="XEW23"/>
       <c r="XEX23"/>
@@ -2991,7 +2984,7 @@
       <c r="XFD23"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="10:16384">
-      <c r="J24" s="31"/>
+      <c r="J24" s="32"/>
       <c r="XEV24"/>
       <c r="XEW24"/>
       <c r="XEX24"/>

</xml_diff>

<commit_message>
se crea modulo trading
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9264" activeTab="3"/>
+    <workbookView windowWidth="22368" windowHeight="9264" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="formula ganancias" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>SALDO INICIAL</t>
   </si>
@@ -133,10 +133,19 @@
     <t>Porcentaje de pérdida</t>
   </si>
   <si>
+    <t>BUY</t>
+  </si>
+  <si>
+    <t>534.95</t>
+  </si>
+  <si>
+    <t>0.06475</t>
+  </si>
+  <si>
     <t>Soporta una varación en contra %</t>
   </si>
   <si>
-    <t>VA 6. Probando 10 automatico y 40 manual</t>
+    <t>VA 6. Probando 10 automatico y X manual</t>
   </si>
   <si>
     <t>peor de los casos</t>
@@ -179,12 +188,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.00000"/>
+    <numFmt numFmtId="178" formatCode="0.000000"/>
+    <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1125,117 +1135,127 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1266,31 +1286,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1302,13 +1322,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1317,19 +1337,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1767,78 +1787,78 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="20.5740740740741" style="70" customWidth="1"/>
-    <col min="2" max="2" width="34.287037037037" style="70" customWidth="1"/>
-    <col min="3" max="3" width="14.1481481481481" style="71" customWidth="1"/>
+    <col min="1" max="1" width="20.5740740740741" style="74" customWidth="1"/>
+    <col min="2" max="2" width="34.287037037037" style="74" customWidth="1"/>
+    <col min="3" max="3" width="14.1481481481481" style="75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A2" s="74">
+      <c r="A2" s="78">
         <v>449.74</v>
       </c>
-      <c r="B2" s="75">
+      <c r="B2" s="79">
         <v>1</v>
       </c>
-      <c r="C2" s="74">
+      <c r="C2" s="78">
         <v>30</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A3" s="76"/>
-      <c r="B3" s="76"/>
+      <c r="A3" s="80"/>
+      <c r="B3" s="80"/>
     </row>
     <row r="4" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="76" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A5" s="75">
+      <c r="A5" s="79">
         <f>POWER(1+(B2/100),C2)*A2</f>
         <v>606.181571181821</v>
       </c>
-      <c r="B5" s="75">
+      <c r="B5" s="79">
         <f>A5-A2</f>
         <v>156.441571181821</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="81"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="78"/>
+      <c r="B7" s="82"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="80" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="76">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="80">
         <f>A9*100/A2</f>
         <v>0.667052074531952</v>
       </c>
@@ -1864,459 +1884,459 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="58.7777777777778" style="40" customWidth="1"/>
-    <col min="2" max="2" width="12.8888888888889" style="40" customWidth="1"/>
-    <col min="3" max="3" width="12.8888888888889" style="40"/>
-    <col min="4" max="4" width="8.44444444444444" style="40" customWidth="1"/>
-    <col min="5" max="5" width="14.7777777777778" style="40" customWidth="1"/>
-    <col min="6" max="6" width="10.8888888888889" style="40" customWidth="1"/>
-    <col min="7" max="7" width="15.6666666666667" style="40" customWidth="1"/>
-    <col min="8" max="8" width="9" style="40" customWidth="1"/>
-    <col min="9" max="9" width="24.8888888888889" style="40" customWidth="1"/>
-    <col min="10" max="10" width="20" style="40" customWidth="1"/>
-    <col min="11" max="16374" width="8.44444444444444" style="40" customWidth="1"/>
-    <col min="16375" max="16375" width="8.44444444444444" style="40"/>
+    <col min="1" max="1" width="58.7777777777778" style="44" customWidth="1"/>
+    <col min="2" max="2" width="12.8888888888889" style="44" customWidth="1"/>
+    <col min="3" max="3" width="12.8888888888889" style="44"/>
+    <col min="4" max="4" width="8.44444444444444" style="44" customWidth="1"/>
+    <col min="5" max="5" width="14.7777777777778" style="44" customWidth="1"/>
+    <col min="6" max="6" width="10.8888888888889" style="44" customWidth="1"/>
+    <col min="7" max="7" width="15.6666666666667" style="44" customWidth="1"/>
+    <col min="8" max="8" width="9" style="44" customWidth="1"/>
+    <col min="9" max="9" width="24.8888888888889" style="44" customWidth="1"/>
+    <col min="10" max="10" width="20" style="44" customWidth="1"/>
+    <col min="11" max="16374" width="8.44444444444444" style="44" customWidth="1"/>
+    <col min="16375" max="16375" width="8.44444444444444" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" s="40" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A1" s="41" t="s">
+    <row r="1" s="44" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="40" customFormat="1" ht="15.15" spans="4:7">
-      <c r="D2" s="43" t="s">
+    <row r="2" s="44" customFormat="1" ht="15.15" spans="4:7">
+      <c r="D2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="40" customFormat="1" spans="1:10">
-      <c r="A3" s="47" t="s">
+    <row r="3" s="44" customFormat="1" spans="1:10">
+      <c r="A3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="52">
         <v>328.24</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="50">
+      <c r="E3" s="54">
         <f>G3/F3</f>
         <v>3607.69371679795</v>
       </c>
-      <c r="F3" s="51">
+      <c r="F3" s="55">
         <v>0.005459</v>
       </c>
-      <c r="G3" s="52">
+      <c r="G3" s="56">
         <f>B8</f>
         <v>19.6944</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="66">
+      <c r="J3" s="70">
         <f>IF(B1="BUY",(J10/I10)-1,(I10/J10)-1)*100</f>
         <v>-1.1306113867434</v>
       </c>
     </row>
-    <row r="4" s="40" customFormat="1" spans="1:10">
-      <c r="A4" s="47" t="s">
+    <row r="4" s="44" customFormat="1" spans="1:10">
+      <c r="A4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="57">
         <f>-B3*$B$19/100</f>
         <v>-32.824</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="58">
         <v>1</v>
       </c>
-      <c r="E4" s="55">
+      <c r="E4" s="59">
         <f t="shared" ref="E4:E11" si="0">E3*(1+$B$6/100)</f>
         <v>4690.00183183733</v>
       </c>
-      <c r="F4" s="56">
+      <c r="F4" s="60">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
         <v>0.005551803</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="56">
         <f t="shared" ref="G4:G17" si="1">E4*F4</f>
         <v>26.03796624</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="66">
+      <c r="J4" s="70">
         <f>E18</f>
         <v>462001.227212826</v>
       </c>
     </row>
-    <row r="5" s="40" customFormat="1" spans="1:10">
-      <c r="A5" s="47" t="s">
+    <row r="5" s="44" customFormat="1" spans="1:10">
+      <c r="A5" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="57">
         <v>1.7</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="58">
         <v>2</v>
       </c>
-      <c r="E5" s="55">
+      <c r="E5" s="59">
         <f t="shared" si="0"/>
         <v>6097.00238138853</v>
       </c>
-      <c r="F5" s="56">
+      <c r="F5" s="60">
         <f t="shared" ref="F5:F12" si="2">IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
         <v>0.005646183651</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="56">
         <f t="shared" si="1"/>
         <v>34.424795165904</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="66">
+      <c r="J5" s="70">
         <f>J4*J10</f>
         <v>2903.20797975916</v>
       </c>
     </row>
-    <row r="6" s="40" customFormat="1" spans="1:10">
-      <c r="A6" s="47" t="s">
+    <row r="6" s="44" customFormat="1" spans="1:10">
+      <c r="A6" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="57">
         <v>30</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="58">
         <v>3</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="59">
         <f t="shared" si="0"/>
         <v>7926.10309580509</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="60">
         <f t="shared" si="2"/>
         <v>0.005742168773067</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="56">
         <f t="shared" si="1"/>
         <v>45.5130216888417</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="66">
+      <c r="J6" s="70">
         <f>J3/100*J4*J10</f>
         <v>-32.824</v>
       </c>
     </row>
-    <row r="7" s="40" customFormat="1" spans="1:10">
-      <c r="A7" s="47" t="s">
+    <row r="7" s="44" customFormat="1" spans="1:10">
+      <c r="A7" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="57">
         <v>10</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="58">
         <v>4</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="59">
         <f t="shared" si="0"/>
         <v>10303.9340245466</v>
       </c>
-      <c r="F7" s="56">
+      <c r="F7" s="60">
         <f t="shared" si="2"/>
         <v>0.00583978564220914</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="56">
         <f t="shared" si="1"/>
         <v>60.1727659748174</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="63">
+      <c r="J7" s="67">
         <f>IF(B1="BUY",(J10/F3)-1,(F3/J10)-1)*100</f>
         <v>-13.1283491593311</v>
       </c>
     </row>
-    <row r="8" s="40" customFormat="1" spans="1:7">
-      <c r="A8" s="47" t="s">
+    <row r="8" s="44" customFormat="1" spans="1:7">
+      <c r="A8" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B8" s="57">
         <f>B3*$B$18/100</f>
         <v>19.6944</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="58">
         <v>5</v>
       </c>
-      <c r="E8" s="55">
+      <c r="E8" s="59">
         <f t="shared" si="0"/>
         <v>13395.1142319106</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="60">
         <f t="shared" si="2"/>
         <v>0.00593906199812669</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="56">
         <f t="shared" si="1"/>
         <v>79.5544138953063</v>
       </c>
     </row>
-    <row r="9" s="40" customFormat="1" spans="1:10">
-      <c r="A9" s="57" t="s">
+    <row r="9" s="44" customFormat="1" spans="1:10">
+      <c r="A9" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="62">
         <v>8</v>
       </c>
-      <c r="D9" s="54">
+      <c r="D9" s="58">
         <v>6</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="59">
         <f t="shared" si="0"/>
         <v>17413.6485014838</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="60">
         <f t="shared" si="2"/>
         <v>0.00604002605209485</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="56">
         <f t="shared" si="1"/>
         <v>105.178890610985</v>
       </c>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="51" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" s="40" customFormat="1" ht="17.4" spans="1:10">
-      <c r="A10" s="57" t="s">
+    <row r="10" s="44" customFormat="1" ht="17.4" spans="1:10">
+      <c r="A10" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="62">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$E$3</f>
         <v>115500.306803206</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="58">
         <v>7</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="59">
         <f t="shared" si="0"/>
         <v>22637.7430519289</v>
       </c>
-      <c r="F10" s="56">
+      <c r="F10" s="60">
         <f>IF($B$1="BUY",F9*(1-$B$5/100),F9*(1+$B$5/100))</f>
         <v>0.00614270649498046</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="56">
         <f t="shared" si="1"/>
         <v>139.057011276782</v>
       </c>
-      <c r="I10" s="67">
+      <c r="I10" s="71">
         <f>G18/E18</f>
         <v>0.00621293583368965</v>
       </c>
-      <c r="J10" s="68">
+      <c r="J10" s="72">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
         <v>0.00628398326401364</v>
       </c>
     </row>
-    <row r="11" s="40" customFormat="1" spans="1:7">
-      <c r="A11" s="57" t="s">
+    <row r="11" s="44" customFormat="1" spans="1:7">
+      <c r="A11" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="62">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$G$3</f>
         <v>630.516174838704</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="58">
         <v>8</v>
       </c>
-      <c r="E11" s="55">
+      <c r="E11" s="59">
         <f t="shared" si="0"/>
         <v>29429.0659675076</v>
       </c>
-      <c r="F11" s="56">
+      <c r="F11" s="60">
         <f>IF($B$1="BUY",F10*(1-$B$5/100),F10*(1+$B$5/100))</f>
         <v>0.00624713250539512</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="56">
         <f t="shared" si="1"/>
         <v>183.847274609034</v>
       </c>
     </row>
-    <row r="12" s="40" customFormat="1" spans="1:7">
-      <c r="A12" s="57" t="s">
+    <row r="12" s="44" customFormat="1" spans="1:7">
+      <c r="A12" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="62">
         <f>B10*3</f>
         <v>346500.920409619</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="58">
         <v>9</v>
       </c>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="52">
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="40" customFormat="1" spans="1:7">
-      <c r="A13" s="57" t="s">
+    <row r="13" s="44" customFormat="1" spans="1:7">
+      <c r="A13" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="58">
+      <c r="B13" s="62">
         <f>B11*3</f>
         <v>1891.54852451611</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="58">
         <v>10</v>
       </c>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="52">
+      <c r="E13" s="59"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" s="40" customFormat="1" spans="1:7">
-      <c r="A14" s="57" t="s">
+    <row r="14" s="44" customFormat="1" spans="1:7">
+      <c r="A14" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="58">
+      <c r="B14" s="62">
         <f>B12+B10</f>
         <v>462001.227212826</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="58">
         <v>11</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="52">
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" s="40" customFormat="1" spans="1:7">
-      <c r="A15" s="57" t="s">
+    <row r="15" s="44" customFormat="1" spans="1:7">
+      <c r="A15" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="58">
+      <c r="B15" s="62">
         <f>B13+B11</f>
         <v>2522.06469935482</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="58">
         <v>12</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="52">
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" s="40" customFormat="1" spans="1:7">
-      <c r="A16" s="57" t="s">
+    <row r="16" s="44" customFormat="1" spans="1:7">
+      <c r="A16" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="58">
+      <c r="B16" s="62">
         <f>B15/B14</f>
         <v>0.005459</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="58">
         <v>13</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="52">
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" s="40" customFormat="1" ht="18.15" spans="1:10">
-      <c r="A17" s="57" t="s">
+    <row r="17" s="44" customFormat="1" ht="18.15" spans="1:10">
+      <c r="A17" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="58">
+      <c r="B17" s="62">
         <f>IF(B1="BUY",((B4/B15)+1)*B16,((B4/-B15)+1)*B16)</f>
         <v>0.00553004743032399</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="64">
         <f>SUM(E3:E15)*3</f>
         <v>346500.920409619</v>
       </c>
-      <c r="F17" s="61">
+      <c r="F17" s="65">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
         <v>0.0062825329229257</v>
       </c>
-      <c r="G17" s="62">
+      <c r="G17" s="66">
         <f t="shared" si="1"/>
         <v>2176.90344029749</v>
       </c>
-      <c r="J17" s="69"/>
-    </row>
-    <row r="18" s="40" customFormat="1" spans="1:10">
-      <c r="A18" s="47" t="s">
+      <c r="J17" s="73"/>
+    </row>
+    <row r="18" s="44" customFormat="1" spans="1:10">
+      <c r="A18" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="63">
+      <c r="B18" s="67">
         <v>6</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="65">
+      <c r="D18" s="68"/>
+      <c r="E18" s="69">
         <f>SUM(E3:E17)</f>
         <v>462001.227212826</v>
       </c>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65">
+      <c r="F18" s="69"/>
+      <c r="G18" s="69">
         <f>SUM(G3:G17)</f>
         <v>2870.38397975916</v>
       </c>
-      <c r="H18" s="64"/>
-      <c r="J18" s="69"/>
-    </row>
-    <row r="19" s="40" customFormat="1" spans="1:10">
-      <c r="A19" s="47" t="s">
+      <c r="H18" s="68"/>
+      <c r="J18" s="73"/>
+    </row>
+    <row r="19" s="44" customFormat="1" spans="1:10">
+      <c r="A19" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="63">
+      <c r="B19" s="67">
         <v>10</v>
       </c>
-      <c r="J19" s="69"/>
-    </row>
-    <row r="20" s="40" customFormat="1" spans="10:10">
-      <c r="J20" s="69"/>
-    </row>
-    <row r="21" s="40" customFormat="1" spans="10:10">
-      <c r="J21" s="69"/>
+      <c r="J19" s="73"/>
+    </row>
+    <row r="20" s="44" customFormat="1" spans="10:10">
+      <c r="J20" s="73"/>
+    </row>
+    <row r="21" s="44" customFormat="1" spans="10:10">
+      <c r="J21" s="73"/>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="69"/>
+      <c r="J22" s="73"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="69"/>
+      <c r="J23" s="73"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="69"/>
+      <c r="J24" s="73"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J6">
@@ -2390,414 +2410,414 @@
   <sheetPr/>
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.8888888888889" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.7777777777778" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.44444444444444" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.5555555555556" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.1111111111111" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.6666666666667" style="2" customWidth="1"/>
-    <col min="8" max="8" width="1.66666666666667" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32.8888888888889" style="2" customWidth="1"/>
-    <col min="10" max="10" width="31.2222222222222" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.44444444444444" style="2" customWidth="1"/>
-    <col min="12" max="12" width="31.2222222222222" style="2" customWidth="1"/>
-    <col min="13" max="16374" width="8.44444444444444" style="2" customWidth="1"/>
-    <col min="16375" max="16375" width="8.44444444444444" style="2"/>
-    <col min="16376" max="16384" width="8.44444444444444" style="1"/>
+    <col min="1" max="1" width="22" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12.8888888888889" style="15" customWidth="1"/>
+    <col min="3" max="3" width="39.7777777777778" style="15" customWidth="1"/>
+    <col min="4" max="4" width="8.44444444444444" style="15" customWidth="1"/>
+    <col min="5" max="5" width="18.5555555555556" style="15" customWidth="1"/>
+    <col min="6" max="6" width="17.1111111111111" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.6666666666667" style="15" customWidth="1"/>
+    <col min="8" max="8" width="1.66666666666667" style="15" customWidth="1"/>
+    <col min="9" max="9" width="32.8888888888889" style="15" customWidth="1"/>
+    <col min="10" max="10" width="31.2222222222222" style="15" customWidth="1"/>
+    <col min="11" max="11" width="8.44444444444444" style="15" customWidth="1"/>
+    <col min="12" max="12" width="31.2222222222222" style="15" customWidth="1"/>
+    <col min="13" max="16374" width="8.44444444444444" style="15" customWidth="1"/>
+    <col min="16375" max="16375" width="8.44444444444444" style="15"/>
+    <col min="16376" max="16384" width="8.44444444444444" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A1" s="16" t="s">
+    <row r="1" s="15" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" s="2" customFormat="1" ht="15.15" spans="4:7">
-      <c r="D2" s="18" t="s">
+      <c r="B1" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" s="15" customFormat="1" ht="15.15" spans="4:7">
+      <c r="D2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:10">
-      <c r="A3" s="5" t="s">
+    <row r="3" s="15" customFormat="1" spans="1:10">
+      <c r="A3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="22">
-        <v>523.5141</v>
-      </c>
-      <c r="D3" s="23" t="s">
+      <c r="B3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="26">
         <f>G3/F3</f>
-        <v>35869.4141829394</v>
-      </c>
-      <c r="F3" s="25">
-        <v>0.005838</v>
-      </c>
-      <c r="G3" s="26">
+        <v>826.177606177606</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="28">
         <f>B8</f>
-        <v>209.40564</v>
-      </c>
-      <c r="I3" s="5" t="s">
+        <v>53.495</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="38">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-3.77016415584495</v>
-      </c>
-    </row>
-    <row r="4" s="2" customFormat="1" spans="1:10">
-      <c r="A4" s="5" t="s">
+        <v>-20.0089023002285</v>
+      </c>
+    </row>
+    <row r="4" s="15" customFormat="1" spans="1:10">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="29">
         <f>-B3*$B$10/100</f>
-        <v>-52.35141</v>
-      </c>
-      <c r="D4" s="27">
+        <v>-53.495</v>
+      </c>
+      <c r="D4" s="30">
         <v>1</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="26">
         <f>E3*(1+$B$6/100)</f>
-        <v>46630.2384378212</v>
-      </c>
-      <c r="F4" s="28">
+        <v>1074.03088803089</v>
+      </c>
+      <c r="F4" s="31">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
-        <v>0.005937246</v>
-      </c>
-      <c r="G4" s="26">
+        <v>0.06364925</v>
+      </c>
+      <c r="G4" s="28">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>276.855196644</v>
-      </c>
-      <c r="I4" s="5" t="s">
+        <v>68.3612605</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="38">
         <f>E18</f>
-        <v>221924.065549846</v>
-      </c>
-    </row>
-    <row r="5" s="2" customFormat="1" spans="1:10">
-      <c r="A5" s="5" t="s">
+        <v>5111.56084942085</v>
+      </c>
+    </row>
+    <row r="5" s="15" customFormat="1" spans="1:10">
+      <c r="A5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="29">
         <v>1.7</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="30">
         <v>2</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="26">
         <f>E4*(1+$B$6/100)</f>
-        <v>60619.3099691675</v>
-      </c>
-      <c r="F5" s="28">
+        <v>1396.24015444015</v>
+      </c>
+      <c r="F5" s="31">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
-        <v>0.006038179182</v>
-      </c>
-      <c r="G5" s="26">
+        <v>0.06256721275</v>
+      </c>
+      <c r="G5" s="28">
         <f t="shared" si="0"/>
-        <v>366.030255483032</v>
-      </c>
-      <c r="I5" s="5" t="s">
+        <v>87.35885479295</v>
+      </c>
+      <c r="I5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="38">
         <f>J4*J10</f>
-        <v>1388.57110290115</v>
-      </c>
-    </row>
-    <row r="6" s="2" customFormat="1" spans="1:10">
-      <c r="A6" s="5" t="s">
+        <v>267.355995832861</v>
+      </c>
+    </row>
+    <row r="6" s="15" customFormat="1" spans="1:10">
+      <c r="A6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="29">
         <v>30</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="30">
         <v>3</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="26">
         <f>E5*(1+$B$6/100)</f>
-        <v>78805.1029599178</v>
-      </c>
-      <c r="F6" s="28">
+        <v>1815.1122007722</v>
+      </c>
+      <c r="F6" s="31">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
-        <v>0.006140828228094</v>
-      </c>
-      <c r="G6" s="26">
+        <v>0.06150357013325</v>
+      </c>
+      <c r="G6" s="28">
         <f t="shared" si="0"/>
-        <v>483.928600774117</v>
-      </c>
-      <c r="I6" s="5" t="s">
+        <v>111.635880539911</v>
+      </c>
+      <c r="I6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="38">
         <f>J3/100*J4*J10</f>
-        <v>-52.35141</v>
-      </c>
-    </row>
-    <row r="7" s="2" customFormat="1" spans="1:10">
-      <c r="A7" s="5" t="s">
+        <v>-53.495</v>
+      </c>
+    </row>
+    <row r="7" s="15" customFormat="1" spans="1:10">
+      <c r="A7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="29">
         <v>10</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="30">
         <v>4</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="26">
+      <c r="E7" s="26"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="9">
+      <c r="I7" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="29">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>7.17651532020362</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="1" spans="1:7">
-      <c r="A8" s="5" t="s">
+        <v>19.2213445104413</v>
+      </c>
+    </row>
+    <row r="8" s="15" customFormat="1" spans="1:7">
+      <c r="A8" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="29">
         <f>B3*$B$9/100</f>
-        <v>209.40564</v>
-      </c>
-      <c r="D8" s="27">
+        <v>53.495</v>
+      </c>
+      <c r="D8" s="30">
         <v>5</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="26">
+      <c r="E8" s="26"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="1" spans="1:10">
-      <c r="A9" s="5" t="s">
+    <row r="9" s="15" customFormat="1" spans="1:10">
+      <c r="A9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="29">
-        <v>40</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="27">
+      <c r="B9" s="32">
+        <v>10</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="30">
         <v>6</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="26">
+      <c r="E9" s="26"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" ht="17.4" spans="1:10">
-      <c r="A10" s="5" t="s">
+    <row r="10" s="15" customFormat="1" ht="17.4" spans="1:10">
+      <c r="A10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="29">
         <v>10</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="30">
         <v>7</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="26">
+      <c r="E10" s="26"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="39">
         <f>G18/E18</f>
-        <v>0.00602106711406215</v>
-      </c>
-      <c r="J10" s="37">
+        <v>0.062769671590472</v>
+      </c>
+      <c r="J10" s="40">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>0.00625696496439349</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="1" spans="4:7">
-      <c r="D11" s="27">
+        <v>0.0523041794294893</v>
+      </c>
+    </row>
+    <row r="11" s="15" customFormat="1" spans="4:7">
+      <c r="D11" s="30">
         <v>8</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="26">
+      <c r="E11" s="26"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" spans="4:7">
-      <c r="D12" s="27">
+    <row r="12" s="15" customFormat="1" spans="4:7">
+      <c r="D12" s="30">
         <v>9</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="26">
+      <c r="E12" s="26"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="1" spans="4:10">
-      <c r="D13" s="27">
+    <row r="13" s="15" customFormat="1" spans="4:10">
+      <c r="D13" s="30">
         <v>10</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="26">
+      <c r="E13" s="26"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" s="2" customFormat="1" spans="4:9">
-      <c r="D14" s="27">
+      <c r="I13" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="41"/>
+    </row>
+    <row r="14" s="15" customFormat="1" spans="4:9">
+      <c r="D14" s="30">
         <v>11</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="26">
+      <c r="E14" s="26"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" s="2" customFormat="1" spans="4:9">
-      <c r="D15" s="27">
+      <c r="I14" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" s="15" customFormat="1" spans="4:9">
+      <c r="D15" s="30">
         <v>12</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="26">
+      <c r="E15" s="26"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="29">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>0.00625696496439349</v>
-      </c>
-    </row>
-    <row r="16" s="2" customFormat="1" spans="4:9">
-      <c r="D16" s="27">
+        <v>0.0523041794294893</v>
+      </c>
+    </row>
+    <row r="16" s="15" customFormat="1" spans="4:9">
+      <c r="D16" s="30">
         <v>13</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="26">
+      <c r="E16" s="26"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" s="2" customFormat="1" ht="18.15" spans="4:10">
-      <c r="D17" s="30" t="s">
+      <c r="I16" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" s="15" customFormat="1" ht="18.15" spans="4:10">
+      <c r="D17" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32">
+      <c r="E17" s="34"/>
+      <c r="F17" s="35">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
-        <v>0.00617562625471986</v>
-      </c>
-      <c r="G17" s="33">
+        <v>0.0611550499024949</v>
+      </c>
+      <c r="G17" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="29">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>3.91787445418774</v>
-      </c>
-      <c r="J17" s="36" t="str">
+        <v>16.6728483610089</v>
+      </c>
+      <c r="J17" s="39" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
-        <v>TIENE QUE BAJAR</v>
-      </c>
-    </row>
-    <row r="18" s="2" customFormat="1" spans="4:8">
-      <c r="D18" s="34"/>
-      <c r="E18" s="34">
+        <v>TIENE QUE SUBIR</v>
+      </c>
+    </row>
+    <row r="18" s="15" customFormat="1" spans="4:8">
+      <c r="D18" s="37"/>
+      <c r="E18" s="37">
         <f>SUM(E3:E17)</f>
-        <v>221924.065549846</v>
-      </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34">
+        <v>5111.56084942085</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37">
         <f>SUM(G3:G17)</f>
-        <v>1336.21969290115</v>
-      </c>
-      <c r="H18" s="34"/>
-    </row>
-    <row r="19" s="2" customFormat="1"/>
-    <row r="20" s="2" customFormat="1"/>
-    <row r="21" s="2" customFormat="1"/>
-    <row r="22" s="2" customFormat="1" spans="16376:16384">
-      <c r="XEV22" s="1"/>
-      <c r="XEW22" s="1"/>
-      <c r="XEX22" s="1"/>
-      <c r="XEY22" s="1"/>
-      <c r="XEZ22" s="1"/>
-      <c r="XFA22" s="1"/>
-      <c r="XFB22" s="1"/>
-      <c r="XFC22" s="1"/>
-      <c r="XFD22" s="1"/>
-    </row>
-    <row r="23" s="2" customFormat="1" spans="16376:16384">
-      <c r="XEV23" s="1"/>
-      <c r="XEW23" s="1"/>
-      <c r="XEX23" s="1"/>
-      <c r="XEY23" s="1"/>
-      <c r="XEZ23" s="1"/>
-      <c r="XFA23" s="1"/>
-      <c r="XFB23" s="1"/>
-      <c r="XFC23" s="1"/>
-      <c r="XFD23" s="1"/>
-    </row>
-    <row r="24" s="2" customFormat="1" spans="16376:16384">
-      <c r="XEV24" s="1"/>
-      <c r="XEW24" s="1"/>
-      <c r="XEX24" s="1"/>
-      <c r="XEY24" s="1"/>
-      <c r="XEZ24" s="1"/>
-      <c r="XFA24" s="1"/>
-      <c r="XFB24" s="1"/>
-      <c r="XFC24" s="1"/>
-      <c r="XFD24" s="1"/>
+        <v>320.850995832861</v>
+      </c>
+      <c r="H18" s="37"/>
+    </row>
+    <row r="19" s="15" customFormat="1"/>
+    <row r="20" s="15" customFormat="1"/>
+    <row r="21" s="15" customFormat="1"/>
+    <row r="22" s="15" customFormat="1" spans="16376:16384">
+      <c r="XEV22" s="16"/>
+      <c r="XEW22" s="16"/>
+      <c r="XEX22" s="16"/>
+      <c r="XEY22" s="16"/>
+      <c r="XEZ22" s="16"/>
+      <c r="XFA22" s="16"/>
+      <c r="XFB22" s="16"/>
+      <c r="XFC22" s="16"/>
+      <c r="XFD22" s="16"/>
+    </row>
+    <row r="23" s="15" customFormat="1" spans="16376:16384">
+      <c r="XEV23" s="16"/>
+      <c r="XEW23" s="16"/>
+      <c r="XEX23" s="16"/>
+      <c r="XEY23" s="16"/>
+      <c r="XEZ23" s="16"/>
+      <c r="XFA23" s="16"/>
+      <c r="XFB23" s="16"/>
+      <c r="XFC23" s="16"/>
+      <c r="XFD23" s="16"/>
+    </row>
+    <row r="24" s="15" customFormat="1" spans="16376:16384">
+      <c r="XEV24" s="16"/>
+      <c r="XEW24" s="16"/>
+      <c r="XEX24" s="16"/>
+      <c r="XEY24" s="16"/>
+      <c r="XEZ24" s="16"/>
+      <c r="XFA24" s="16"/>
+      <c r="XFB24" s="16"/>
+      <c r="XFC24" s="16"/>
+      <c r="XFD24" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2874,21 +2894,23 @@
   <sheetPr/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.44444444444444" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.66666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.4444444444444" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.88888888888889" style="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.66666666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4444444444444" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.1111111111111" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.4444444444444" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1111111111111" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="11" width="12.8888888888889" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.2222222222222" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.2222222222222" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7777777777778" style="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
@@ -2906,31 +2928,31 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2938,65 +2960,65 @@
         <v>13</v>
       </c>
       <c r="B3" s="6">
-        <v>519.93</v>
+        <v>538.63</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="8">
-        <v>209</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.005838</v>
-      </c>
-      <c r="G3" s="9">
+        <v>53</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1678</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.006075</v>
+      </c>
+      <c r="G3" s="8">
         <f t="shared" ref="G3:G6" si="0">E3/F3</f>
-        <v>35799.9314833847</v>
-      </c>
-      <c r="H3" s="10">
+        <v>276213.991769547</v>
+      </c>
+      <c r="H3" s="9">
         <f>IF(A2="BUY",((I3/J3)-1)*-100,((I3/J3)-1)*100)</f>
-        <v>-1.59439164696152</v>
-      </c>
-      <c r="I3" s="10">
+        <v>-3.31640742129513</v>
+      </c>
+      <c r="I3" s="9">
         <f>SUM(E3:E4)/SUM(G3:G4)</f>
-        <v>0.0880635586394634</v>
-      </c>
-      <c r="J3" s="10">
+        <v>0.006075</v>
+      </c>
+      <c r="J3" s="9">
         <f>IF(A2="BUY",((B4/SUM(E3:E4))+1)*I3,((B4/-SUM(E3:E4))+1)*I3)</f>
-        <v>0.0894903858767154</v>
-      </c>
-      <c r="K3" s="13">
+        <v>0.00587999539630512</v>
+      </c>
+      <c r="K3" s="12">
         <f>H3/100*SUM(G3:G4)*J3</f>
-        <v>-51.993</v>
+        <v>-53.8630000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <f>-B3*10/100</f>
-        <v>-51.993</v>
+        <v>-53.863</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E4" s="6">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6">
-        <v>4.69</v>
-      </c>
-      <c r="G4" s="9">
+        <v>0.006031</v>
+      </c>
+      <c r="G4" s="8">
         <f t="shared" si="0"/>
-        <v>639.658848614072</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="3:10">
       <c r="C5" s="2"/>
@@ -3013,20 +3035,20 @@
       <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="9">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="8">
         <f>IF(A2="BUY",((F3/J6)-1)*-100,((F3/J6)-1)*100)</f>
-        <v>1.35416666666666</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="8">
-        <v>0.00576</v>
-      </c>
-      <c r="K6" s="15">
-        <f>H6/100*SUM(G3)*J6</f>
-        <v>2.79239465570399</v>
+        <v>0.654129190515129</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="6">
+        <v>0.006115</v>
+      </c>
+      <c r="K6" s="14">
+        <f>H6/100*SUM(G3:G4)*J6</f>
+        <v>11.0485596707819</v>
       </c>
     </row>
     <row r="7" spans="3:11">

</xml_diff>

<commit_message>
se vuelve a 6 de entrada
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -142,7 +142,7 @@
     <t>Soporta una varación en contra %</t>
   </si>
   <si>
-    <t>VA 6. Probando 9 automatico y X manual</t>
+    <t>Automáico 6. manual 19</t>
   </si>
   <si>
     <t>peor de los casos</t>
@@ -188,9 +188,9 @@
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="0.000000"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="26">
@@ -249,9 +249,24 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,7 +288,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,14 +318,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -310,6 +340,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -318,14 +364,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,48 +378,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -393,7 +393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,12 +420,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -438,6 +432,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -450,169 +450,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,6 +877,26 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -902,30 +916,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -937,15 +927,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -968,32 +949,45 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1005,170 +999,170 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1220,9 +1214,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1238,7 +1229,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1307,10 +1298,10 @@
     <xf numFmtId="179" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1331,7 +1322,7 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1784,78 +1775,78 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.5740740740741" style="72" customWidth="1"/>
-    <col min="2" max="2" width="34.287037037037" style="72" customWidth="1"/>
-    <col min="3" max="3" width="14.1481481481481" style="73" customWidth="1"/>
+    <col min="1" max="1" width="20.5740740740741" style="71" customWidth="1"/>
+    <col min="2" max="2" width="34.287037037037" style="71" customWidth="1"/>
+    <col min="3" max="3" width="14.1481481481481" style="72" customWidth="1"/>
     <col min="4" max="4" width="21.8888888888889" customWidth="1"/>
     <col min="5" max="5" width="17.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="73" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A2" s="76">
+      <c r="A2" s="75">
         <v>650</v>
       </c>
-      <c r="B2" s="77">
+      <c r="B2" s="76">
         <v>0.82</v>
       </c>
-      <c r="C2" s="76">
+      <c r="C2" s="75">
         <v>30</v>
       </c>
-      <c r="D2" s="78">
+      <c r="D2" s="77">
         <f>POWER(1+(B2/100),C2)*A2</f>
         <v>830.451262564387</v>
       </c>
-      <c r="E2" s="78">
+      <c r="E2" s="77">
         <f>D2-A2</f>
         <v>180.451262564387</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="72"/>
     </row>
     <row r="4" ht="19.5" customHeight="1"/>
     <row r="5" ht="19.5" customHeight="1"/>
     <row r="6" ht="19.5" customHeight="1" spans="1:2">
-      <c r="A6" s="79"/>
-      <c r="B6" s="79"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="80"/>
+      <c r="B7" s="79"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="80" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="82">
+      <c r="A9" s="81">
         <v>4.5</v>
       </c>
-      <c r="B9" s="81">
+      <c r="B9" s="80">
         <f>A9*100/A2</f>
         <v>0.692307692307692</v>
       </c>
@@ -1881,459 +1872,459 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="58.7777777777778" style="43" customWidth="1"/>
-    <col min="2" max="2" width="12.8888888888889" style="43" customWidth="1"/>
-    <col min="3" max="3" width="12.8888888888889" style="43"/>
-    <col min="4" max="4" width="8.44444444444444" style="43" customWidth="1"/>
-    <col min="5" max="5" width="14.7777777777778" style="43" customWidth="1"/>
-    <col min="6" max="6" width="10.8888888888889" style="43" customWidth="1"/>
-    <col min="7" max="7" width="15.6666666666667" style="43" customWidth="1"/>
-    <col min="8" max="8" width="9" style="43" customWidth="1"/>
-    <col min="9" max="9" width="24.8888888888889" style="43" customWidth="1"/>
-    <col min="10" max="10" width="20" style="43" customWidth="1"/>
-    <col min="11" max="16374" width="8.44444444444444" style="43" customWidth="1"/>
-    <col min="16375" max="16375" width="8.44444444444444" style="43"/>
+    <col min="1" max="1" width="58.7777777777778" style="42" customWidth="1"/>
+    <col min="2" max="2" width="12.8888888888889" style="42" customWidth="1"/>
+    <col min="3" max="3" width="12.8888888888889" style="42"/>
+    <col min="4" max="4" width="8.44444444444444" style="42" customWidth="1"/>
+    <col min="5" max="5" width="14.7777777777778" style="42" customWidth="1"/>
+    <col min="6" max="6" width="10.8888888888889" style="42" customWidth="1"/>
+    <col min="7" max="7" width="15.6666666666667" style="42" customWidth="1"/>
+    <col min="8" max="8" width="9" style="42" customWidth="1"/>
+    <col min="9" max="9" width="24.8888888888889" style="42" customWidth="1"/>
+    <col min="10" max="10" width="20" style="42" customWidth="1"/>
+    <col min="11" max="16374" width="8.44444444444444" style="42" customWidth="1"/>
+    <col min="16375" max="16375" width="8.44444444444444" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" s="43" customFormat="1" ht="15.75" spans="1:2">
-      <c r="A1" s="44" t="s">
+    <row r="1" s="42" customFormat="1" ht="15.75" spans="1:2">
+      <c r="A1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="43" customFormat="1" ht="15.15" spans="4:7">
-      <c r="D2" s="46" t="s">
+    <row r="2" s="42" customFormat="1" ht="15.15" spans="4:7">
+      <c r="D2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="43" customFormat="1" spans="1:10">
-      <c r="A3" s="50" t="s">
+    <row r="3" s="42" customFormat="1" spans="1:10">
+      <c r="A3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="50">
         <v>328.24</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="53">
+      <c r="E3" s="52">
         <f>G3/F3</f>
         <v>3607.69371679795</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="53">
         <v>0.005459</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="54">
         <f>B8</f>
         <v>19.6944</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="68">
+      <c r="J3" s="67">
         <f>IF(B1="BUY",(J10/I10)-1,(I10/J10)-1)*100</f>
         <v>-1.1306113867434</v>
       </c>
     </row>
-    <row r="4" s="43" customFormat="1" spans="1:10">
-      <c r="A4" s="50" t="s">
+    <row r="4" s="42" customFormat="1" spans="1:10">
+      <c r="A4" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="55">
         <f>-B3*$B$19/100</f>
         <v>-32.824</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="56">
         <v>1</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="57">
         <f t="shared" ref="E4:E11" si="0">E3*(1+$B$6/100)</f>
         <v>4690.00183183733</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="58">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
         <v>0.005551803</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="54">
         <f t="shared" ref="G4:G17" si="1">E4*F4</f>
         <v>26.03796624</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="67">
         <f>E18</f>
         <v>462001.227212826</v>
       </c>
     </row>
-    <row r="5" s="43" customFormat="1" spans="1:10">
-      <c r="A5" s="50" t="s">
+    <row r="5" s="42" customFormat="1" spans="1:10">
+      <c r="A5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="55">
         <v>1.7</v>
       </c>
-      <c r="D5" s="57">
+      <c r="D5" s="56">
         <v>2</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="57">
         <f t="shared" si="0"/>
         <v>6097.00238138853</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="58">
         <f t="shared" ref="F5:F12" si="2">IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
         <v>0.005646183651</v>
       </c>
-      <c r="G5" s="55">
+      <c r="G5" s="54">
         <f t="shared" si="1"/>
         <v>34.424795165904</v>
       </c>
-      <c r="I5" s="50" t="s">
+      <c r="I5" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="67">
         <f>J4*J10</f>
         <v>2903.20797975916</v>
       </c>
     </row>
-    <row r="6" s="43" customFormat="1" spans="1:10">
-      <c r="A6" s="50" t="s">
+    <row r="6" s="42" customFormat="1" spans="1:10">
+      <c r="A6" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="55">
         <v>30</v>
       </c>
-      <c r="D6" s="57">
+      <c r="D6" s="56">
         <v>3</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="57">
         <f t="shared" si="0"/>
         <v>7926.10309580509</v>
       </c>
-      <c r="F6" s="59">
+      <c r="F6" s="58">
         <f t="shared" si="2"/>
         <v>0.005742168773067</v>
       </c>
-      <c r="G6" s="55">
+      <c r="G6" s="54">
         <f t="shared" si="1"/>
         <v>45.5130216888417</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="I6" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="67">
         <f>J3/100*J4*J10</f>
         <v>-32.824</v>
       </c>
     </row>
-    <row r="7" s="43" customFormat="1" spans="1:10">
-      <c r="A7" s="50" t="s">
+    <row r="7" s="42" customFormat="1" spans="1:10">
+      <c r="A7" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="56">
+      <c r="B7" s="55">
         <v>10</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="56">
         <v>4</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="57">
         <f t="shared" si="0"/>
         <v>10303.9340245466</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="58">
         <f t="shared" si="2"/>
         <v>0.00583978564220914</v>
       </c>
-      <c r="G7" s="55">
+      <c r="G7" s="54">
         <f t="shared" si="1"/>
         <v>60.1727659748174</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="65">
+      <c r="J7" s="64">
         <f>IF(B1="BUY",(J10/F3)-1,(F3/J10)-1)*100</f>
         <v>-13.1283491593311</v>
       </c>
     </row>
-    <row r="8" s="43" customFormat="1" spans="1:7">
-      <c r="A8" s="50" t="s">
+    <row r="8" s="42" customFormat="1" spans="1:7">
+      <c r="A8" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="56">
+      <c r="B8" s="55">
         <f>B3*$B$18/100</f>
         <v>19.6944</v>
       </c>
-      <c r="D8" s="57">
+      <c r="D8" s="56">
         <v>5</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="57">
         <f t="shared" si="0"/>
         <v>13395.1142319106</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="58">
         <f t="shared" si="2"/>
         <v>0.00593906199812669</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8" s="54">
         <f t="shared" si="1"/>
         <v>79.5544138953063</v>
       </c>
     </row>
-    <row r="9" s="43" customFormat="1" spans="1:10">
-      <c r="A9" s="60" t="s">
+    <row r="9" s="42" customFormat="1" spans="1:10">
+      <c r="A9" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="61">
+      <c r="B9" s="60">
         <v>8</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="56">
         <v>6</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="57">
         <f t="shared" si="0"/>
         <v>17413.6485014838</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="58">
         <f t="shared" si="2"/>
         <v>0.00604002605209485</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="54">
         <f t="shared" si="1"/>
         <v>105.178890610985</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="50" t="s">
+      <c r="J9" s="49" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" s="43" customFormat="1" ht="17.4" spans="1:10">
-      <c r="A10" s="60" t="s">
+    <row r="10" s="42" customFormat="1" ht="17.4" spans="1:10">
+      <c r="A10" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="61">
+      <c r="B10" s="60">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$E$3</f>
         <v>115500.306803206</v>
       </c>
-      <c r="D10" s="57">
+      <c r="D10" s="56">
         <v>7</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="57">
         <f t="shared" si="0"/>
         <v>22637.7430519289</v>
       </c>
-      <c r="F10" s="59">
+      <c r="F10" s="58">
         <f>IF($B$1="BUY",F9*(1-$B$5/100),F9*(1+$B$5/100))</f>
         <v>0.00614270649498046</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="54">
         <f t="shared" si="1"/>
         <v>139.057011276782</v>
       </c>
-      <c r="I10" s="69">
+      <c r="I10" s="68">
         <f>G18/E18</f>
         <v>0.00621293583368965</v>
       </c>
-      <c r="J10" s="70">
+      <c r="J10" s="69">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
         <v>0.00628398326401364</v>
       </c>
     </row>
-    <row r="11" s="43" customFormat="1" spans="1:7">
-      <c r="A11" s="60" t="s">
+    <row r="11" s="42" customFormat="1" spans="1:7">
+      <c r="A11" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="61">
+      <c r="B11" s="60">
         <f>((1-POWER(1+$B$6/100,$B$9+1))/(1-(1+$B$6/100)))*$G$3</f>
         <v>630.516174838704</v>
       </c>
-      <c r="D11" s="57">
+      <c r="D11" s="56">
         <v>8</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="57">
         <f t="shared" si="0"/>
         <v>29429.0659675076</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="58">
         <f>IF($B$1="BUY",F10*(1-$B$5/100),F10*(1+$B$5/100))</f>
         <v>0.00624713250539512</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="54">
         <f t="shared" si="1"/>
         <v>183.847274609034</v>
       </c>
     </row>
-    <row r="12" s="43" customFormat="1" spans="1:7">
-      <c r="A12" s="60" t="s">
+    <row r="12" s="42" customFormat="1" spans="1:7">
+      <c r="A12" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="61">
+      <c r="B12" s="60">
         <f>B10*3</f>
         <v>346500.920409619</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="56">
         <v>9</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="55">
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="43" customFormat="1" spans="1:7">
-      <c r="A13" s="60" t="s">
+    <row r="13" s="42" customFormat="1" spans="1:7">
+      <c r="A13" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="61">
+      <c r="B13" s="60">
         <f>B11*3</f>
         <v>1891.54852451611</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="56">
         <v>10</v>
       </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="55">
+      <c r="E13" s="57"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" s="43" customFormat="1" spans="1:7">
-      <c r="A14" s="60" t="s">
+    <row r="14" s="42" customFormat="1" spans="1:7">
+      <c r="A14" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="61">
+      <c r="B14" s="60">
         <f>B12+B10</f>
         <v>462001.227212826</v>
       </c>
-      <c r="D14" s="57">
+      <c r="D14" s="56">
         <v>11</v>
       </c>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="55">
+      <c r="E14" s="57"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" s="43" customFormat="1" spans="1:7">
-      <c r="A15" s="60" t="s">
+    <row r="15" s="42" customFormat="1" spans="1:7">
+      <c r="A15" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="61">
+      <c r="B15" s="60">
         <f>B13+B11</f>
         <v>2522.06469935482</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="56">
         <v>12</v>
       </c>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="55">
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" s="43" customFormat="1" spans="1:7">
-      <c r="A16" s="60" t="s">
+    <row r="16" s="42" customFormat="1" spans="1:7">
+      <c r="A16" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="61">
+      <c r="B16" s="60">
         <f>B15/B14</f>
         <v>0.005459</v>
       </c>
-      <c r="D16" s="57">
+      <c r="D16" s="56">
         <v>13</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="55">
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" s="43" customFormat="1" ht="18.15" spans="1:10">
-      <c r="A17" s="60" t="s">
+    <row r="17" s="42" customFormat="1" ht="18.15" spans="1:10">
+      <c r="A17" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="61">
+      <c r="B17" s="60">
         <f>IF(B1="BUY",((B4/B15)+1)*B16,((B4/-B15)+1)*B16)</f>
         <v>0.00553004743032399</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <f>SUM(E3:E15)*3</f>
         <v>346500.920409619</v>
       </c>
-      <c r="F17" s="63">
+      <c r="F17" s="62">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
         <v>0.0062825329229257</v>
       </c>
-      <c r="G17" s="64">
+      <c r="G17" s="63">
         <f t="shared" si="1"/>
         <v>2176.90344029749</v>
       </c>
-      <c r="J17" s="71"/>
-    </row>
-    <row r="18" s="43" customFormat="1" spans="1:10">
-      <c r="A18" s="50" t="s">
+      <c r="J17" s="70"/>
+    </row>
+    <row r="18" s="42" customFormat="1" spans="1:10">
+      <c r="A18" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="65">
+      <c r="B18" s="64">
         <v>6</v>
       </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="67">
+      <c r="D18" s="65"/>
+      <c r="E18" s="66">
         <f>SUM(E3:E17)</f>
         <v>462001.227212826</v>
       </c>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67">
+      <c r="F18" s="66"/>
+      <c r="G18" s="66">
         <f>SUM(G3:G17)</f>
         <v>2870.38397975916</v>
       </c>
-      <c r="H18" s="66"/>
-      <c r="J18" s="71"/>
-    </row>
-    <row r="19" s="43" customFormat="1" spans="1:10">
-      <c r="A19" s="50" t="s">
+      <c r="H18" s="65"/>
+      <c r="J18" s="70"/>
+    </row>
+    <row r="19" s="42" customFormat="1" spans="1:10">
+      <c r="A19" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="65">
+      <c r="B19" s="64">
         <v>10</v>
       </c>
-      <c r="J19" s="71"/>
-    </row>
-    <row r="20" s="43" customFormat="1" spans="10:10">
-      <c r="J20" s="71"/>
-    </row>
-    <row r="21" s="43" customFormat="1" spans="10:10">
-      <c r="J21" s="71"/>
+      <c r="J19" s="70"/>
+    </row>
+    <row r="20" s="42" customFormat="1" spans="10:10">
+      <c r="J20" s="70"/>
+    </row>
+    <row r="21" s="42" customFormat="1" spans="10:10">
+      <c r="J21" s="70"/>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="71"/>
+      <c r="J22" s="70"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="71"/>
+      <c r="J23" s="70"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="71"/>
+      <c r="J24" s="70"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J6">
@@ -2408,7 +2399,7 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2464,21 +2455,21 @@
       </c>
       <c r="E3" s="25">
         <f>G3/F3</f>
-        <v>39.3728802153432</v>
+        <v>26.2485868102288</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="27">
         <f>B8</f>
-        <v>58.5081</v>
+        <v>39.0054</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="36">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-14.8303924336603</v>
+        <v>-20.7099083127727</v>
       </c>
     </row>
     <row r="4" s="14" customFormat="1" spans="1:10">
@@ -2494,7 +2485,7 @@
       </c>
       <c r="E4" s="25">
         <f>E3*(1+$B$6/100)</f>
-        <v>51.1847442799462</v>
+        <v>34.1231628532974</v>
       </c>
       <c r="F4" s="30">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
@@ -2502,14 +2493,14 @@
       </c>
       <c r="G4" s="27">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>77.35355901</v>
+        <v>51.56903934</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="36">
         <f>E18</f>
-        <v>243.600009892328</v>
+        <v>162.400006594886</v>
       </c>
     </row>
     <row r="5" s="14" customFormat="1" spans="1:10">
@@ -2524,7 +2515,7 @@
       </c>
       <c r="E5" s="25">
         <f>E4*(1+$B$6/100)</f>
-        <v>66.54016756393</v>
+        <v>44.3601117092867</v>
       </c>
       <c r="F5" s="30">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
@@ -2532,14 +2523,14 @@
       </c>
       <c r="G5" s="27">
         <f t="shared" si="0"/>
-        <v>102.269140367121</v>
+        <v>68.179426911414</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="36">
         <f>J4*J10</f>
-        <v>438.349829856492</v>
+        <v>313.902886570994</v>
       </c>
     </row>
     <row r="6" s="14" customFormat="1" spans="1:10">
@@ -2554,7 +2545,7 @@
       </c>
       <c r="E6" s="25">
         <f>E5*(1+$B$6/100)</f>
-        <v>86.502217833109</v>
+        <v>57.6681452220727</v>
       </c>
       <c r="F6" s="30">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
@@ -2562,12 +2553,12 @@
       </c>
       <c r="G6" s="27">
         <f t="shared" si="0"/>
-        <v>135.210030479371</v>
+        <v>90.1400203195805</v>
       </c>
       <c r="I6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="36">
         <f>J3/100*J4*J10</f>
         <v>-65.009</v>
       </c>
@@ -2593,7 +2584,7 @@
       </c>
       <c r="J7" s="28">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>21.0945872631665</v>
+        <v>30.0739885166909</v>
       </c>
     </row>
     <row r="8" s="14" customFormat="1" spans="1:7">
@@ -2602,7 +2593,7 @@
       </c>
       <c r="B8" s="28">
         <f>B3*$B$9/100</f>
-        <v>58.5081</v>
+        <v>39.0054</v>
       </c>
       <c r="D8" s="29">
         <v>5</v>
@@ -2618,8 +2609,8 @@
       <c r="A9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="31">
-        <v>9</v>
+      <c r="B9" s="28">
+        <v>6</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>41</v>
@@ -2656,13 +2647,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="37">
         <f>G18/E18</f>
         <v>1.53259776147591</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="38">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>1.79946556673065</v>
+        <v>1.93289946935803</v>
       </c>
     </row>
     <row r="11" s="14" customFormat="1" spans="4:7">
@@ -2697,10 +2688,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="40"/>
+      <c r="J13" s="39"/>
     </row>
     <row r="14" s="14" customFormat="1" spans="4:9">
       <c r="D14" s="29">
@@ -2712,7 +2703,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="40" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2728,7 +2719,7 @@
       </c>
       <c r="I15" s="28">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>1.79946556673065</v>
+        <v>1.93289946935803</v>
       </c>
     </row>
     <row r="16" s="14" customFormat="1" spans="4:9">
@@ -2741,44 +2732,44 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="41" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" s="14" customFormat="1" ht="18.15" spans="4:10">
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34">
+      <c r="E17" s="32"/>
+      <c r="F17" s="33">
         <f>IF(B1="BUY",MIN(F3:F16)*(1-($B$5/3)/100),MAX(F3:F16)*(1+($B$5/3)/100))</f>
         <v>1.5719391254734</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I17" s="28">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>17.4127753519455</v>
-      </c>
-      <c r="J17" s="38" t="str">
+        <v>26.1191630279183</v>
+      </c>
+      <c r="J17" s="37" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
         <v>TIENE QUE BAJAR</v>
       </c>
     </row>
     <row r="18" s="14" customFormat="1" spans="4:8">
-      <c r="D18" s="36"/>
-      <c r="E18" s="36">
+      <c r="D18" s="35"/>
+      <c r="E18" s="35">
         <f>SUM(E3:E17)</f>
-        <v>243.600009892328</v>
-      </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36">
+        <v>162.400006594886</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35">
         <f>SUM(G3:G17)</f>
-        <v>373.340829856492</v>
-      </c>
-      <c r="H18" s="36"/>
+        <v>248.893886570994</v>
+      </c>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" s="14" customFormat="1"/>
     <row r="20" s="14" customFormat="1"/>

</xml_diff>

<commit_message>
divisor. Se maneja en creaactualizatps
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>SALDO INICIAL</t>
   </si>
@@ -133,13 +133,16 @@
     <t>Porcentaje de pérdida</t>
   </si>
   <si>
-    <t>650.09</t>
+    <t>639</t>
   </si>
   <si>
     <t>1.4860</t>
   </si>
   <si>
     <t>Soporta una varación en contra %</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>Automáico 6. manual 19</t>
@@ -2399,7 +2402,7 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2455,14 +2458,14 @@
       </c>
       <c r="E3" s="25">
         <f>G3/F3</f>
-        <v>26.2485868102288</v>
+        <v>25.8008075370121</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="27">
         <f>B8</f>
-        <v>39.0054</v>
+        <v>38.34</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>15</v>
@@ -2478,14 +2481,14 @@
       </c>
       <c r="B4" s="28">
         <f>-B3*$B$10/100</f>
-        <v>-65.009</v>
+        <v>-63.9</v>
       </c>
       <c r="D4" s="29">
         <v>1</v>
       </c>
       <c r="E4" s="25">
         <f>E3*(1+$B$6/100)</f>
-        <v>34.1231628532974</v>
+        <v>33.5410497981158</v>
       </c>
       <c r="F4" s="30">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
@@ -2493,14 +2496,14 @@
       </c>
       <c r="G4" s="27">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>51.56903934</v>
+        <v>50.689314</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="36">
         <f>E18</f>
-        <v>162.400006594886</v>
+        <v>159.629596231494</v>
       </c>
     </row>
     <row r="5" s="14" customFormat="1" spans="1:10">
@@ -2515,7 +2518,7 @@
       </c>
       <c r="E5" s="25">
         <f>E4*(1+$B$6/100)</f>
-        <v>44.3601117092867</v>
+        <v>43.6033647375505</v>
       </c>
       <c r="F5" s="30">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
@@ -2523,14 +2526,14 @@
       </c>
       <c r="G5" s="27">
         <f t="shared" si="0"/>
-        <v>68.179426911414</v>
+        <v>67.0163420394</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="36">
         <f>J4*J10</f>
-        <v>313.902886570994</v>
+        <v>308.547961849691</v>
       </c>
     </row>
     <row r="6" s="14" customFormat="1" spans="1:10">
@@ -2545,7 +2548,7 @@
       </c>
       <c r="E6" s="25">
         <f>E5*(1+$B$6/100)</f>
-        <v>57.6681452220727</v>
+        <v>56.6843741588156</v>
       </c>
       <c r="F6" s="30">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
@@ -2553,14 +2556,14 @@
       </c>
       <c r="G6" s="27">
         <f t="shared" si="0"/>
-        <v>90.1400203195805</v>
+        <v>88.6023058102908</v>
       </c>
       <c r="I6" s="22" t="s">
         <v>21</v>
       </c>
       <c r="J6" s="36">
         <f>J3/100*J4*J10</f>
-        <v>-65.009</v>
+        <v>-63.9</v>
       </c>
     </row>
     <row r="7" s="14" customFormat="1" spans="1:10">
@@ -2593,7 +2596,7 @@
       </c>
       <c r="B8" s="28">
         <f>B3*$B$9/100</f>
-        <v>39.0054</v>
+        <v>38.34</v>
       </c>
       <c r="D8" s="29">
         <v>5</v>
@@ -2609,11 +2612,11 @@
       <c r="A9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="28">
-        <v>6</v>
+      <c r="B9" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="29">
         <v>6</v>
@@ -2689,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J13" s="39"/>
     </row>
@@ -2704,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" s="14" customFormat="1" spans="4:9">
@@ -2733,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" s="14" customFormat="1" ht="18.15" spans="4:10">
@@ -2762,12 +2765,12 @@
       <c r="D18" s="35"/>
       <c r="E18" s="35">
         <f>SUM(E3:E17)</f>
-        <v>162.400006594886</v>
+        <v>159.629596231494</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35">
         <f>SUM(G3:G17)</f>
-        <v>248.893886570994</v>
+        <v>244.647961849691</v>
       </c>
       <c r="H18" s="35"/>
     </row>
@@ -2883,7 +2886,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2922,25 +2925,25 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2952,33 +2955,33 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="6">
-        <v>1400</v>
+        <v>491</v>
       </c>
       <c r="F3" s="6">
-        <v>1.4967</v>
+        <v>6.18</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" ref="G3:G6" si="0">E3/F3</f>
-        <v>935.391193960045</v>
+        <v>79.4498381877023</v>
       </c>
       <c r="H3" s="9">
         <f>IF(A2="BUY",((I3/J3)-1)*-100,((I3/J3)-1)*100)</f>
-        <v>-1.83334882826552</v>
+        <v>-11.4514389592027</v>
       </c>
       <c r="I3" s="9">
         <f>SUM(E3:E4)/SUM(G3:G4)</f>
-        <v>1.51031858476198</v>
+        <v>6.18</v>
       </c>
       <c r="J3" s="9">
         <f>IF(A2="BUY",((B4/SUM(E3:E4))+1)*I3,((B4/-SUM(E3:E4))+1)*I3)</f>
-        <v>1.53852511696645</v>
+        <v>6.97922126272912</v>
       </c>
       <c r="K3" s="11">
         <f>H3/100*SUM(G3:G4)*J3</f>
-        <v>-63.4979999999999</v>
+        <v>-63.498</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2991,17 +2994,17 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="6">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6">
-        <v>1.52</v>
+        <v>6.368</v>
       </c>
       <c r="G4" s="8">
         <f t="shared" si="0"/>
-        <v>1315.78947368421</v>
+        <v>0</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -3028,15 +3031,15 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8">
         <f>IF(A2="BUY",((F3/J6)-1)*-100,((F3/J6)-1)*100)</f>
-        <v>0.449664429530205</v>
+        <v>1.42786804529789</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="6">
-        <v>1.49</v>
+        <v>6.093</v>
       </c>
       <c r="K6" s="13">
         <f>H6/100*SUM(G3:G4)*J6</f>
-        <v>15.0829104732166</v>
+        <v>6.91213592233011</v>
       </c>
     </row>
     <row r="7" spans="3:11">

</xml_diff>

<commit_message>
vuelvo con el tp a 50%
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -133,7 +133,7 @@
     <t>Porcentaje de pérdida</t>
   </si>
   <si>
-    <t>654</t>
+    <t>772.37</t>
   </si>
   <si>
     <t>1.4860</t>
@@ -189,12 +189,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000000"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="0.00000"/>
+    <numFmt numFmtId="176" formatCode="0.00000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.000000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -253,14 +253,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,28 +274,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -305,7 +283,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,17 +329,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -373,9 +352,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,25 +435,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,145 +603,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,20 +884,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -913,6 +910,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -942,21 +948,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -967,6 +958,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -984,188 +984,188 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1220,7 +1220,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1274,31 +1274,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1310,10 +1310,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1322,19 +1322,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2402,7 +2402,7 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2458,14 +2458,14 @@
       </c>
       <c r="E3" s="25">
         <f>G3/F3</f>
-        <v>83.6204576043069</v>
+        <v>98.7552489905787</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="27">
         <f>B8</f>
-        <v>124.26</v>
+        <v>146.7503</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>15</v>
@@ -2481,14 +2481,14 @@
       </c>
       <c r="B4" s="28">
         <f>-B3*$B$10/100</f>
-        <v>-65.4</v>
+        <v>-77.237</v>
       </c>
       <c r="D4" s="29">
         <v>1</v>
       </c>
       <c r="E4" s="25">
         <f>E3*(1+$B$6/100)</f>
-        <v>108.706594885599</v>
+        <v>128.381823687752</v>
       </c>
       <c r="F4" s="30">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
@@ -2496,14 +2496,14 @@
       </c>
       <c r="G4" s="27">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>164.284146</v>
+        <v>194.01857163</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="36">
         <f>E18</f>
-        <v>517.359771197847</v>
+        <v>610.998725504711</v>
       </c>
     </row>
     <row r="5" s="14" customFormat="1" spans="1:10">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="E5" s="25">
         <f>E4*(1+$B$6/100)</f>
-        <v>141.318573351279</v>
+        <v>166.896370794078</v>
       </c>
       <c r="F5" s="30">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
@@ -2526,14 +2526,14 @@
       </c>
       <c r="G5" s="27">
         <f t="shared" si="0"/>
-        <v>217.2000694266</v>
+        <v>256.511953552023</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="36">
         <f>J4*J10</f>
-        <v>858.304427215508</v>
+        <v>1013.65227897315</v>
       </c>
     </row>
     <row r="6" s="14" customFormat="1" spans="1:10">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="E6" s="25">
         <f>E5*(1+$B$6/100)</f>
-        <v>183.714145356662</v>
+        <v>216.965282032302</v>
       </c>
       <c r="F6" s="30">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
@@ -2556,14 +2556,14 @@
       </c>
       <c r="G6" s="27">
         <f t="shared" si="0"/>
-        <v>287.160211788908</v>
+        <v>339.13445379113</v>
       </c>
       <c r="I6" s="22" t="s">
         <v>21</v>
       </c>
       <c r="J6" s="36">
         <f>J3/100*J4*J10</f>
-        <v>-65.4</v>
+        <v>-77.237</v>
       </c>
     </row>
     <row r="7" s="14" customFormat="1" spans="1:10">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B8" s="28">
         <f>B3*$B$9/100</f>
-        <v>124.26</v>
+        <v>146.7503</v>
       </c>
       <c r="D8" s="29">
         <v>5</v>
@@ -2765,12 +2765,12 @@
       <c r="D18" s="35"/>
       <c r="E18" s="35">
         <f>SUM(E3:E17)</f>
-        <v>517.359771197847</v>
+        <v>610.998725504711</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35">
         <f>SUM(G3:G17)</f>
-        <v>792.904427215508</v>
+        <v>936.415278973153</v>
       </c>
       <c r="H18" s="35"/>
     </row>
@@ -2886,7 +2886,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2951,7 +2951,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="6">
-        <v>654</v>
+        <v>772.37</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H3" s="9">
         <f>IF(A2="BUY",((I3/J3)-1)*-100,((I3/J3)-1)*100)</f>
-        <v>-2.0028174189992</v>
+        <v>-2.3567718782621</v>
       </c>
       <c r="I3" s="9">
         <f>SUM(E3:E4)/SUM(G3:G4)</f>
@@ -2977,11 +2977,11 @@
       </c>
       <c r="J3" s="9">
         <f>IF(A2="BUY",((B4/SUM(E3:E4))+1)*I3,((B4/-SUM(E3:E4))+1)*I3)</f>
-        <v>0.190558398018744</v>
+        <v>0.1912491678348</v>
       </c>
       <c r="K3" s="11">
         <f>H3/100*SUM(G3:G4)*J3</f>
-        <v>-65.4</v>
+        <v>-77.2370000000006</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="B4" s="8">
         <f>-B3*10/100</f>
-        <v>-65.4</v>
+        <v>-77.237</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">

</xml_diff>

<commit_message>
solo 2 valores de profit
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9264" activeTab="2"/>
+    <workbookView windowWidth="22368" windowHeight="9264" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="formula ganancias" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
     <t>Porcentaje de pérdida</t>
   </si>
   <si>
-    <t>772.37</t>
+    <t>771.17</t>
   </si>
   <si>
     <t>1.4860</t>
@@ -189,12 +189,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="0.00000"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="0.000000"/>
+    <numFmt numFmtId="179" formatCode="0.00000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -259,10 +259,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -274,24 +283,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,6 +308,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,22 +344,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -368,12 +360,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -395,6 +388,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -441,97 +441,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,73 +609,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -880,21 +880,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -934,6 +919,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -987,12 +987,12 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1002,170 +1002,170 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1220,7 +1220,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1274,31 +1274,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1310,10 +1310,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1322,19 +1322,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2401,8 +2401,8 @@
   <sheetPr/>
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2458,14 +2458,14 @@
       </c>
       <c r="E3" s="25">
         <f>G3/F3</f>
-        <v>98.7552489905787</v>
+        <v>98.6018169582773</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="27">
         <f>B8</f>
-        <v>146.7503</v>
+        <v>146.5223</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>15</v>
@@ -2481,14 +2481,14 @@
       </c>
       <c r="B4" s="28">
         <f>-B3*$B$10/100</f>
-        <v>-77.237</v>
+        <v>-77.117</v>
       </c>
       <c r="D4" s="29">
         <v>1</v>
       </c>
       <c r="E4" s="25">
         <f>E3*(1+$B$6/100)</f>
-        <v>128.381823687752</v>
+        <v>128.18236204576</v>
       </c>
       <c r="F4" s="30">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
@@ -2496,14 +2496,14 @@
       </c>
       <c r="G4" s="27">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>194.01857163</v>
+        <v>193.71713283</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="36">
         <f>E18</f>
-        <v>610.998725504711</v>
+        <v>610.049441520861</v>
       </c>
     </row>
     <row r="5" s="14" customFormat="1" spans="1:10">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="E5" s="25">
         <f>E4*(1+$B$6/100)</f>
-        <v>166.896370794078</v>
+        <v>166.637070659489</v>
       </c>
       <c r="F5" s="30">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
@@ -2526,14 +2526,14 @@
       </c>
       <c r="G5" s="27">
         <f t="shared" si="0"/>
-        <v>256.511953552023</v>
+        <v>256.113421314543</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="36">
         <f>J4*J10</f>
-        <v>1013.65227897315</v>
+        <v>1012.0774084645</v>
       </c>
     </row>
     <row r="6" s="14" customFormat="1" spans="1:10">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="E6" s="25">
         <f>E5*(1+$B$6/100)</f>
-        <v>216.965282032302</v>
+        <v>216.628191857335</v>
       </c>
       <c r="F6" s="30">
         <f>IF($B$1="BUY",F5*(1-$B$5/100),F5*(1+$B$5/100))</f>
@@ -2556,14 +2556,14 @@
       </c>
       <c r="G6" s="27">
         <f t="shared" si="0"/>
-        <v>339.13445379113</v>
+        <v>338.607554319957</v>
       </c>
       <c r="I6" s="22" t="s">
         <v>21</v>
       </c>
       <c r="J6" s="36">
         <f>J3/100*J4*J10</f>
-        <v>-77.237</v>
+        <v>-77.117</v>
       </c>
     </row>
     <row r="7" s="14" customFormat="1" spans="1:10">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B8" s="28">
         <f>B3*$B$9/100</f>
-        <v>146.7503</v>
+        <v>146.5223</v>
       </c>
       <c r="D8" s="29">
         <v>5</v>
@@ -2765,12 +2765,12 @@
       <c r="D18" s="35"/>
       <c r="E18" s="35">
         <f>SUM(E3:E17)</f>
-        <v>610.998725504711</v>
+        <v>610.049441520861</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35">
         <f>SUM(G3:G17)</f>
-        <v>936.415278973153</v>
+        <v>934.9604084645</v>
       </c>
       <c r="H18" s="35"/>
     </row>
@@ -2885,7 +2885,7 @@
   <sheetPr/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2951,7 +2951,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="6">
-        <v>772.37</v>
+        <v>771.17</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H3" s="9">
         <f>IF(A2="BUY",((I3/J3)-1)*-100,((I3/J3)-1)*100)</f>
-        <v>-2.3567718782621</v>
+        <v>-2.35319642234317</v>
       </c>
       <c r="I3" s="9">
         <f>SUM(E3:E4)/SUM(G3:G4)</f>
@@ -2977,11 +2977,11 @@
       </c>
       <c r="J3" s="9">
         <f>IF(A2="BUY",((B4/SUM(E3:E4))+1)*I3,((B4/-SUM(E3:E4))+1)*I3)</f>
-        <v>0.1912491678348</v>
+        <v>0.191242165015003</v>
       </c>
       <c r="K3" s="11">
         <f>H3/100*SUM(G3:G4)*J3</f>
-        <v>-77.2370000000006</v>
+        <v>-77.1169999999999</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="B4" s="8">
         <f>-B3*10/100</f>
-        <v>-77.237</v>
+        <v>-77.117</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">

</xml_diff>

<commit_message>
SE TOMAN TODAS LAS OPORTUNIDADES
</commit_message>
<xml_diff>
--- a/old/FORMULAss.xlsx
+++ b/old/FORMULAss.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>SALDO INICIAL</t>
   </si>
@@ -133,7 +133,7 @@
     <t>Porcentaje de pérdida</t>
   </si>
   <si>
-    <t>813</t>
+    <t>823</t>
   </si>
   <si>
     <t>1.4860</t>
@@ -142,7 +142,7 @@
     <t>Soporta una varación en contra %</t>
   </si>
   <si>
-    <t>6</t>
+    <t>26</t>
   </si>
   <si>
     <t>Automáico 6. manual 19</t>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>distancia entre posicion y precio</t>
-  </si>
-  <si>
-    <t>BUY</t>
   </si>
   <si>
     <t>Size</t>
@@ -2405,7 +2402,7 @@
   <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44444444444444" defaultRowHeight="14.4"/>
@@ -2461,21 +2458,21 @@
       </c>
       <c r="E3" s="25">
         <f>G3/F3</f>
-        <v>32.8263795423957</v>
+        <v>143.99730820996</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="27">
         <f>B8</f>
-        <v>48.78</v>
+        <v>213.98</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="36">
         <f>IF(B1="BUY",((I10/J10)-1)*-100,((I10/J10)-1)*100)</f>
-        <v>-29.052631068355</v>
+        <v>-8.63399354807185</v>
       </c>
     </row>
     <row r="4" s="14" customFormat="1" spans="1:10">
@@ -2484,14 +2481,14 @@
       </c>
       <c r="B4" s="28">
         <f>-B3*$B$10/100</f>
-        <v>-81.3</v>
+        <v>-82.3</v>
       </c>
       <c r="D4" s="29">
         <v>1</v>
       </c>
       <c r="E4" s="25">
         <f>E3*(1+$B$6/100)</f>
-        <v>42.6742934051144</v>
+        <v>187.196500672948</v>
       </c>
       <c r="F4" s="30">
         <f>IF($B$1="BUY",F3*(1-$B$5/100),F3*(1+$B$5/100))</f>
@@ -2499,14 +2496,14 @@
       </c>
       <c r="G4" s="27">
         <f t="shared" ref="G4:G17" si="0">E4*F4</f>
-        <v>64.492038</v>
+        <v>282.902958</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="36">
         <f>E18</f>
-        <v>130.977254374159</v>
+        <v>574.549259757739</v>
       </c>
     </row>
     <row r="5" s="14" customFormat="1" spans="1:10">
@@ -2521,7 +2518,7 @@
       </c>
       <c r="E5" s="25">
         <f>E4*(1+$B$6/100)</f>
-        <v>55.4765814266487</v>
+        <v>243.355450874832</v>
       </c>
       <c r="F5" s="30">
         <f>IF($B$1="BUY",F4*(1-$B$5/100),F4*(1+$B$5/100))</f>
@@ -2529,14 +2526,14 @@
       </c>
       <c r="G5" s="27">
         <f t="shared" si="0"/>
-        <v>85.2649234398</v>
+        <v>374.0260007718</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="36">
         <f>J4*J10</f>
-        <v>279.8369614398</v>
+        <v>953.2089587718</v>
       </c>
     </row>
     <row r="6" s="14" customFormat="1" spans="1:10">
@@ -2560,7 +2557,7 @@
       </c>
       <c r="J6" s="36">
         <f>J3/100*J4*J10</f>
-        <v>-81.3</v>
+        <v>-82.3000000000001</v>
       </c>
     </row>
     <row r="7" s="14" customFormat="1" spans="1:10">
@@ -2584,7 +2581,7 @@
       </c>
       <c r="J7" s="28">
         <f>IF(B1="BUY",(((J10/F3)-1)*-1),(J10/F3)-1)*100</f>
-        <v>43.7773202172097</v>
+        <v>11.6457091382302</v>
       </c>
     </row>
     <row r="8" s="14" customFormat="1" spans="1:7">
@@ -2593,7 +2590,7 @@
       </c>
       <c r="B8" s="28">
         <f>B3*$B$9/100</f>
-        <v>48.78</v>
+        <v>213.98</v>
       </c>
       <c r="D8" s="29">
         <v>5</v>
@@ -2653,7 +2650,7 @@
       </c>
       <c r="J10" s="38">
         <f>IF(B1="BUY",((B4/G18)+1)*I10,((B4/-G18)+1)*I10)</f>
-        <v>2.13653097842774</v>
+        <v>1.6590552377941</v>
       </c>
     </row>
     <row r="11" s="14" customFormat="1" spans="4:7">
@@ -2719,7 +2716,7 @@
       </c>
       <c r="I15" s="28">
         <f>IF(B1="BUY",F3*(1-(J7)/100),F3*(1+(J7)/100))</f>
-        <v>2.13653097842774</v>
+        <v>1.6590552377941</v>
       </c>
     </row>
     <row r="16" s="14" customFormat="1" spans="4:9">
@@ -2751,7 +2748,7 @@
       </c>
       <c r="I17" s="28">
         <f>IF(B1="BUY",(((I15/I10)-1)*-1),((I15/I10)-1))*100</f>
-        <v>40.94955388176</v>
+        <v>9.44989704963695</v>
       </c>
       <c r="J17" s="37" t="str">
         <f>IF(B1="BUY","TIENE QUE SUBIR","TIENE QUE BAJAR")</f>
@@ -2762,12 +2759,12 @@
       <c r="D18" s="35"/>
       <c r="E18" s="35">
         <f>SUM(E3:E17)</f>
-        <v>130.977254374159</v>
+        <v>574.549259757739</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35">
         <f>SUM(G3:G17)</f>
-        <v>198.5369614398</v>
+        <v>870.9089587718</v>
       </c>
       <c r="H18" s="35"/>
     </row>
@@ -2883,7 +2880,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2916,31 +2913,31 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2948,37 +2945,37 @@
         <v>13</v>
       </c>
       <c r="B3" s="6">
-        <v>809</v>
+        <v>824</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="6">
-        <v>905</v>
+        <v>1042</v>
       </c>
       <c r="F3" s="6">
-        <v>0.216</v>
+        <v>1.0189641</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" ref="G3:G6" si="0">E3/F3</f>
-        <v>4189.81481481481</v>
+        <v>1022.60717526751</v>
       </c>
       <c r="H3" s="9">
         <f>IF(A2="BUY",((I3/J3)-1)*-100,((I3/J3)-1)*100)</f>
-        <v>-9.81676980948916</v>
+        <v>-7.32835289932408</v>
       </c>
       <c r="I3" s="9">
         <f>SUM(E3:E4)/SUM(G3:G4)</f>
-        <v>0.216</v>
+        <v>1.0189641</v>
       </c>
       <c r="J3" s="9">
         <f>IF(A2="BUY",((B4/SUM(E3:E4))+1)*I3,((B4/-SUM(E3:E4))+1)*I3)</f>
-        <v>0.196691270718232</v>
+        <v>1.09954245109405</v>
       </c>
       <c r="K3" s="11">
         <f>H3/100*SUM(G3:G4)*J3</f>
-        <v>-80.9000000000001</v>
+        <v>-82.3999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2987,17 +2984,17 @@
       </c>
       <c r="B4" s="8">
         <f>-B3*10/100</f>
-        <v>-80.9</v>
+        <v>-82.4</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="6">
         <v>0</v>
       </c>
       <c r="F4" s="6">
-        <v>0.189</v>
+        <v>1.05</v>
       </c>
       <c r="G4" s="8">
         <f t="shared" si="0"/>
@@ -3028,15 +3025,15 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8">
         <f>IF(A2="BUY",((F3/J6)-1)*-100,((F3/J6)-1)*100)</f>
-        <v>0.689655172413794</v>
+        <v>0.708054951571468</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="6">
-        <v>0.2175</v>
+        <v>1.0118</v>
       </c>
       <c r="K6" s="13">
         <f>H6/100*SUM(G3:G4)*J6</f>
-        <v>6.28472222222223</v>
+        <v>7.32606006433409</v>
       </c>
     </row>
     <row r="7" spans="3:11">

</xml_diff>